<commit_message>
update analysis, translaste data
</commit_message>
<xml_diff>
--- a/Analyses/main study/outputs/01_dataPreperation/final/networkIndicators_post_final.xlsx
+++ b/Analyses/main study/outputs/01_dataPreperation/final/networkIndicators_post_final.xlsx
@@ -1442,652 +1442,652 @@
     <t>9199241d-cdbf-443e-9053-9e5ad8551802</t>
   </si>
   <si>
-    <t>643cff9260890a3b38e3130d</t>
-  </si>
-  <si>
-    <t>656606a373aba3beafcf538a</t>
-  </si>
-  <si>
-    <t>64f1dbf275e44ffd381b8985</t>
-  </si>
-  <si>
-    <t>646dc14e28531e7b267adb50</t>
-  </si>
-  <si>
-    <t>6441a254a387409ea3ef316b</t>
-  </si>
-  <si>
-    <t>5bbbdca68f3bd70001e713ef</t>
-  </si>
-  <si>
-    <t>653a743f3112ad79e0e9c2f3</t>
-  </si>
-  <si>
-    <t>651d020dba3016438d70773e</t>
-  </si>
-  <si>
-    <t>65216081309ddac9a26e5d3a</t>
-  </si>
-  <si>
-    <t>65270eab7c3eeb6fda130ee8</t>
-  </si>
-  <si>
-    <t>6516d8dd04d46519d544f6ae</t>
-  </si>
-  <si>
-    <t>6521568f62c55df10e59dc9a</t>
-  </si>
-  <si>
-    <t>656b4e172906db15e11ebce5</t>
-  </si>
-  <si>
-    <t>6557747cc5cd5cb46edfe6c6</t>
-  </si>
-  <si>
-    <t>6554d5f1a5b42aea269aa82a</t>
-  </si>
-  <si>
-    <t>6533fca6a20c492a2baf878e</t>
-  </si>
-  <si>
-    <t>6510335c6c5ba95f95c5af89</t>
-  </si>
-  <si>
-    <t>654baf4c709dd68c04a8b09a</t>
-  </si>
-  <si>
-    <t>65674ca014879b38a634b741</t>
-  </si>
-  <si>
-    <t>65413d7a889c08941364abb6</t>
-  </si>
-  <si>
-    <t>6505b19314eb42b422d59509</t>
-  </si>
-  <si>
-    <t>653fbb7899638eb02212c25b</t>
-  </si>
-  <si>
-    <t>64e220abe394efe48bfe28f8</t>
-  </si>
-  <si>
-    <t>6557923d4a9cc0c7d81cd60d</t>
-  </si>
-  <si>
-    <t>607079a28a504f214dfd77b8</t>
-  </si>
-  <si>
-    <t>6503144bcc000df7879d9637</t>
-  </si>
-  <si>
-    <t>6543cbb6e554d07ea95a1db8</t>
-  </si>
-  <si>
-    <t>6517299ba3d7cde45394692a</t>
-  </si>
-  <si>
-    <t>644ac0e41a2fabcf5d563f20</t>
-  </si>
-  <si>
-    <t>6554d26c5dae0f7aa6a24b19</t>
-  </si>
-  <si>
-    <t>5fff0b0bcbc37a5f5928ed26</t>
-  </si>
-  <si>
-    <t>651311510abdac9c5b9c6c4b</t>
-  </si>
-  <si>
-    <t>615416df060f5730a1d4e113</t>
-  </si>
-  <si>
-    <t>656e5185676b397a22189d00</t>
-  </si>
-  <si>
-    <t>65410ad762a7e3c570b6273c</t>
-  </si>
-  <si>
-    <t>6516d284e2e240661699806c</t>
-  </si>
-  <si>
-    <t>64fdee2b969a06603ae3226d</t>
-  </si>
-  <si>
-    <t>5f738b981a302b0d6d6405aa</t>
-  </si>
-  <si>
-    <t>65465caa5dcdb76a16d563b3</t>
-  </si>
-  <si>
-    <t>5dea808cce8d8d19f5424b21</t>
-  </si>
-  <si>
-    <t>65170df8def70fb50be8068e</t>
-  </si>
-  <si>
-    <t>63c0157fbc63b6511d336764</t>
-  </si>
-  <si>
-    <t>615452aaabb932ada88ef3ca</t>
-  </si>
-  <si>
-    <t>5e6a3e3d265930022e81c70b</t>
-  </si>
-  <si>
-    <t>6524e0ef44178670528207b7</t>
-  </si>
-  <si>
-    <t>6572deb3c978dbcde1a8106c</t>
-  </si>
-  <si>
-    <t>6516d540a78298897619e273</t>
-  </si>
-  <si>
-    <t>651f003609736cc7a85d4328</t>
-  </si>
-  <si>
-    <t>653916355709faa03524b0df</t>
-  </si>
-  <si>
-    <t>638e2654a069e9c741d21ce3</t>
-  </si>
-  <si>
-    <t>65391c7ecf65866247606910</t>
-  </si>
-  <si>
-    <t>65674761184f5501367c963d</t>
-  </si>
-  <si>
-    <t>631f3fde43831da4ae27754b</t>
-  </si>
-  <si>
-    <t>63eb7c1abdbdf911ec1201ab</t>
-  </si>
-  <si>
-    <t>6518e333bba544ebf169f41b</t>
-  </si>
-  <si>
-    <t>650c02a928518783a1b963fd</t>
-  </si>
-  <si>
-    <t>5be95af71ca46b0001862746</t>
-  </si>
-  <si>
-    <t>5b0a869f1e55760001b93fa3</t>
-  </si>
-  <si>
-    <t>654b4a0e936bc8d3c57bfbf0</t>
-  </si>
-  <si>
-    <t>65182c5a0cadd3291661b9e0</t>
-  </si>
-  <si>
-    <t>6526a2a40ce1608344c552bc</t>
-  </si>
-  <si>
-    <t>5be454621effe60001cbf290</t>
-  </si>
-  <si>
-    <t>6529483ef2abe408d574860a</t>
-  </si>
-  <si>
-    <t>64ef6d994d6b1f11074bdfcf</t>
-  </si>
-  <si>
-    <t>5d43c606773d8b00016eaa8a</t>
-  </si>
-  <si>
-    <t>60fe7985ba99343ad0b893b7</t>
-  </si>
-  <si>
-    <t>60513ec07ee46769ed029be4</t>
-  </si>
-  <si>
-    <t>6516d4259c30f249ac643d4b</t>
-  </si>
-  <si>
-    <t>6516d321ac5a66a7aef87507</t>
-  </si>
-  <si>
-    <t>6565f2ba13586fa869dd3b28</t>
-  </si>
-  <si>
-    <t>63c54053d14cc248d3bffebd</t>
-  </si>
-  <si>
-    <t>650c42b04e90f6c176d20f48</t>
-  </si>
-  <si>
-    <t>611ba1976cd48fdde1f9edd3</t>
-  </si>
-  <si>
-    <t>59a426b35fd74b0001abfa4f</t>
-  </si>
-  <si>
-    <t>5bf4033ff719c9000153d38e</t>
-  </si>
-  <si>
-    <t>6480b160d51d051b42f67b3d</t>
-  </si>
-  <si>
-    <t>5aad4225811b2000016f6ed1</t>
-  </si>
-  <si>
-    <t>5e9f28299286a70a21369a87</t>
-  </si>
-  <si>
-    <t>655f017761462616d393ed61</t>
-  </si>
-  <si>
-    <t>6458f51ce9dfaceaf66923b7</t>
-  </si>
-  <si>
-    <t>6568ad4a9ad5cefdb6e70dc7</t>
-  </si>
-  <si>
-    <t>6516f474d21c67a9a5bbb712</t>
-  </si>
-  <si>
-    <t>604d17eb4931a500d6e0a3d3</t>
-  </si>
-  <si>
-    <t>655906b1346b2b209cd19772</t>
-  </si>
-  <si>
-    <t>64369636de5954c6029e89b4</t>
-  </si>
-  <si>
-    <t>6519d311acb10856b9cff800</t>
-  </si>
-  <si>
-    <t>6571d06ee2f60c04ca775e78</t>
-  </si>
-  <si>
-    <t>653671ae2ac8d502b52b1bb3</t>
-  </si>
-  <si>
-    <t>60fd15295d6b2a3711cafbd2</t>
-  </si>
-  <si>
-    <t>651758fd2a0e6965260a89fc</t>
-  </si>
-  <si>
-    <t>6427068bce4fc1aa335ad025</t>
-  </si>
-  <si>
-    <t>5dd08cf019eecb169dc131ba</t>
-  </si>
-  <si>
-    <t>627bbf69ab2788507bc421a2</t>
-  </si>
-  <si>
-    <t>5ebe6e4a226f3b1c53cd0626</t>
-  </si>
-  <si>
-    <t>63d02bd28e37a2abe1006c61</t>
-  </si>
-  <si>
-    <t>652d1a0830b934d1643b80c5</t>
-  </si>
-  <si>
-    <t>6517e9bc213462dc2254bd24</t>
-  </si>
-  <si>
-    <t>650ff7a187874a12d765b5ef</t>
-  </si>
-  <si>
-    <t>65170d2924df1aca5e1b075b</t>
-  </si>
-  <si>
-    <t>6517283ed2294dbc8561979d</t>
-  </si>
-  <si>
-    <t>65367487f0d1c1607d3665c9</t>
-  </si>
-  <si>
-    <t>654e379c8578beb912aee2ff</t>
-  </si>
-  <si>
-    <t>6039b30f86b21c537bfb9448</t>
-  </si>
-  <si>
-    <t>656c50a4c053d63a280ad6d0</t>
-  </si>
-  <si>
-    <t>6536973604f263f3c70495bf</t>
-  </si>
-  <si>
-    <t>654a45fc528885d395cd5cab</t>
-  </si>
-  <si>
-    <t>5c9fd46cfd19090012b4ac8b</t>
-  </si>
-  <si>
-    <t>646219bb0b91a6f3327e39fb</t>
-  </si>
-  <si>
-    <t>6384d76e3da4c98dc29e390b</t>
-  </si>
-  <si>
-    <t>6521569041baced19add37bc</t>
-  </si>
-  <si>
-    <t>5da727bfc2a70a0011a128e0</t>
-  </si>
-  <si>
-    <t>5de81f0edb424d7965702d2d</t>
-  </si>
-  <si>
-    <t>64f1e6cd05138cd766340792</t>
-  </si>
-  <si>
-    <t>64fee13e6324ea4884bcc9db</t>
-  </si>
-  <si>
-    <t>6505c50f48dfd793a7787b8a</t>
-  </si>
-  <si>
-    <t>63eb38339e72d01818aeb71b</t>
-  </si>
-  <si>
-    <t>65313217ba43953a5e06fcae</t>
-  </si>
-  <si>
-    <t>6571e455af2e5eae9adea54a</t>
-  </si>
-  <si>
-    <t>6123c4f8e486767a57db9afe</t>
-  </si>
-  <si>
-    <t>650c2a3e5ae50ab8668448de</t>
-  </si>
-  <si>
-    <t>653d060aaf01dfc1443ad299</t>
-  </si>
-  <si>
-    <t>650a5cc55e8ddf8bae0b81fb</t>
-  </si>
-  <si>
-    <t>640b7f3428d986ad3da9ebcf</t>
-  </si>
-  <si>
-    <t>653bb9c18fa69d049372d45f</t>
-  </si>
-  <si>
-    <t>5ed0f0bb34177d0009582f38</t>
-  </si>
-  <si>
-    <t>604d26915c5dc2a98d18c7fd</t>
-  </si>
-  <si>
-    <t>5dd5855018beb6544df7f797</t>
-  </si>
-  <si>
-    <t>63c33a62f56571779a295a6f</t>
-  </si>
-  <si>
-    <t>653bbdbd990bb0039d427925</t>
-  </si>
-  <si>
-    <t>5f298b2b7823df0a46e25d81</t>
-  </si>
-  <si>
-    <t>6559eb6c636ef499cb5e1f85</t>
-  </si>
-  <si>
-    <t>653be644c2d5f2b6d285699e</t>
-  </si>
-  <si>
-    <t>5edc8e2eaa0f2295a0fcef85</t>
-  </si>
-  <si>
-    <t>646b607e88557c2ff4f0de85</t>
-  </si>
-  <si>
-    <t>5fb42f807e81960acbfdb22e</t>
-  </si>
-  <si>
-    <t>62ed054b4bf00da20ea22dc2</t>
-  </si>
-  <si>
-    <t>629756625dc7cf458e36151f</t>
-  </si>
-  <si>
-    <t>650455b9cde6207c1ebd732b</t>
-  </si>
-  <si>
-    <t>603a80b01bb75f608c3dbb0d</t>
-  </si>
-  <si>
-    <t>65410b3f1de864e712bb267d</t>
-  </si>
-  <si>
-    <t>62c42b020ddc9564f77e2e24</t>
-  </si>
-  <si>
-    <t>6053d1011605ac6f3164bc99</t>
-  </si>
-  <si>
-    <t>65170641ac562bb61fb8e647</t>
-  </si>
-  <si>
-    <t>652680aaf06124cc46807a30</t>
-  </si>
-  <si>
-    <t>655b4ea3ab2c763e739cb199</t>
-  </si>
-  <si>
-    <t>6525ab791fb0b3aaf866d7c7</t>
-  </si>
-  <si>
-    <t>591a1f4800a5650001276188</t>
-  </si>
-  <si>
-    <t>655c754ee949a617a358b8c5</t>
-  </si>
-  <si>
-    <t>6304a2502fbdd7626ed9c2ac</t>
-  </si>
-  <si>
-    <t>652fe4a08d5ecae18fc4fe31</t>
-  </si>
-  <si>
-    <t>6543aeb6dd91d965fc3df508</t>
-  </si>
-  <si>
-    <t>6536b3467fc9c8f7dbabcf51</t>
-  </si>
-  <si>
-    <t>653d07d22dd9d12c6e7b8082</t>
-  </si>
-  <si>
-    <t>6538ef6ac2e74e7d85a136ca</t>
-  </si>
-  <si>
-    <t>63b6be975097f6e31872fc0e</t>
-  </si>
-  <si>
-    <t>6544ea06d33e1704f993f76f</t>
-  </si>
-  <si>
-    <t>60207652caa62b6a34ff96dc</t>
-  </si>
-  <si>
-    <t>610905a730569ffea2fbdd0b</t>
-  </si>
-  <si>
-    <t>5a942689b5e2110001c67d93</t>
-  </si>
-  <si>
-    <t>645b8b2128bbb68d29778068</t>
-  </si>
-  <si>
-    <t>6516d3c10cc8996984d514f4</t>
-  </si>
-  <si>
-    <t>604b169fe4b7991ec08da3a6</t>
-  </si>
-  <si>
-    <t>6569ffc2439eb88f22d4e8bc</t>
-  </si>
-  <si>
-    <t>5fcf9f17f5a7c20ba38e9cc9</t>
-  </si>
-  <si>
-    <t>64ff13ded28d546281ffb6b5</t>
-  </si>
-  <si>
-    <t>6544fd5d0fb2eaaf83e2ddc9</t>
-  </si>
-  <si>
-    <t>63fd0b137e38c72ea19176aa</t>
-  </si>
-  <si>
-    <t>653a50254cd0995ce9fed45e</t>
-  </si>
-  <si>
-    <t>651ec655d2ef1a3ba8e64470</t>
-  </si>
-  <si>
-    <t>5a7fab56f49c9a0001f3549e</t>
-  </si>
-  <si>
-    <t>6554d1f1fda70c02063f51bd</t>
-  </si>
-  <si>
-    <t>6552628d0dfe6b458c390708</t>
-  </si>
-  <si>
-    <t>5b21646bdf28a7000166f4dc</t>
-  </si>
-  <si>
-    <t>6568ccd0468b7384e18af74b</t>
-  </si>
-  <si>
-    <t>6480b08b4e783b4c327cf4a8</t>
-  </si>
-  <si>
-    <t>6505e770a24e4561f219381e</t>
-  </si>
-  <si>
-    <t>653adf50c2b4d95715fa0383</t>
-  </si>
-  <si>
-    <t>63dfd4fb58435f30c7e5b04b</t>
-  </si>
-  <si>
-    <t>65526268c396c0c75dcefdf2</t>
-  </si>
-  <si>
-    <t>6560c1ff0b97f1d037b3c2dd</t>
-  </si>
-  <si>
-    <t>6521ac4e830108f7281e8644</t>
-  </si>
-  <si>
-    <t>606b94352e103bc54d43321b</t>
-  </si>
-  <si>
-    <t>64e74f0c7ba1863371602661</t>
-  </si>
-  <si>
-    <t>6532825749ca31d35c5cc482</t>
-  </si>
-  <si>
-    <t>63b87d2c9edd47ad702413a1</t>
-  </si>
-  <si>
-    <t>5f32d5f107d49607c3f6cf7a</t>
-  </si>
-  <si>
-    <t>6429682ff18d08f9eed7d9e7</t>
-  </si>
-  <si>
-    <t>643c243ff0ef4cb25c20a392</t>
-  </si>
-  <si>
-    <t>63cf5dcd6dbd0452632b58bb</t>
-  </si>
-  <si>
-    <t>617082143afa2b9f049f8b3b</t>
-  </si>
-  <si>
-    <t>647e2500ac34cb60b8e1348d</t>
-  </si>
-  <si>
-    <t>61574c44d4bd510e680f9d7a</t>
-  </si>
-  <si>
-    <t>6516ff4cda6f1e36fd05b1cc</t>
-  </si>
-  <si>
-    <t>5f4cde1cbfcaa81fc4dbf57d</t>
-  </si>
-  <si>
-    <t>6561ff666e87c03638f8fb11</t>
-  </si>
-  <si>
-    <t>64539733186ad1764e4c2b74</t>
-  </si>
-  <si>
-    <t>63cfbea470ab1bba9db30082</t>
-  </si>
-  <si>
-    <t>65034478b7a228b2bdfdca5c</t>
-  </si>
-  <si>
-    <t>6526b4db08c36959a00e69c4</t>
-  </si>
-  <si>
-    <t>6537d0d238ce085ea079c318</t>
-  </si>
-  <si>
-    <t>6570908f385d595d5df25c68</t>
-  </si>
-  <si>
-    <t>652156df21a8be7bb4c6f4e7</t>
-  </si>
-  <si>
-    <t>616b2d4ff5ffb8b86c08661b</t>
-  </si>
-  <si>
-    <t>65426792dac360c44e4908a7</t>
-  </si>
-  <si>
-    <t>65772f25af9bdd7c3ae47af5</t>
-  </si>
-  <si>
-    <t>652d2a7b11d97787933195c6</t>
-  </si>
-  <si>
-    <t>6516d85620c0017a8db27afc</t>
-  </si>
-  <si>
-    <t>654a76de0874380f590ca432</t>
-  </si>
-  <si>
-    <t>63eb514012c203a7a2146262</t>
-  </si>
-  <si>
-    <t>6046b9bf731b0611fe4d0159</t>
-  </si>
-  <si>
-    <t>5f5494aa76d6147f7ca89533</t>
-  </si>
-  <si>
-    <t>5e5fbff6de7bcc2fc7f396db</t>
-  </si>
-  <si>
-    <t>613b5e02f007dc6d30164fb3</t>
-  </si>
-  <si>
-    <t>64f1e17e5439f81a8eade6c2</t>
-  </si>
-  <si>
-    <t>5bceffb6a69cc50001d42ea5</t>
-  </si>
-  <si>
-    <t>60fd19bb0d1f1d54adccc4fa</t>
+    <t>643cff9260890a3b38e3130d_post</t>
+  </si>
+  <si>
+    <t>656606a373aba3beafcf538a_post</t>
+  </si>
+  <si>
+    <t>64f1dbf275e44ffd381b8985_post</t>
+  </si>
+  <si>
+    <t>646dc14e28531e7b267adb50_post</t>
+  </si>
+  <si>
+    <t>6441a254a387409ea3ef316b_post</t>
+  </si>
+  <si>
+    <t>5bbbdca68f3bd70001e713ef_post</t>
+  </si>
+  <si>
+    <t>653a743f3112ad79e0e9c2f3_post</t>
+  </si>
+  <si>
+    <t>651d020dba3016438d70773e_post</t>
+  </si>
+  <si>
+    <t>65216081309ddac9a26e5d3a_post</t>
+  </si>
+  <si>
+    <t>65270eab7c3eeb6fda130ee8_post</t>
+  </si>
+  <si>
+    <t>6516d8dd04d46519d544f6ae_post</t>
+  </si>
+  <si>
+    <t>6521568f62c55df10e59dc9a_post</t>
+  </si>
+  <si>
+    <t>656b4e172906db15e11ebce5_post</t>
+  </si>
+  <si>
+    <t>6557747cc5cd5cb46edfe6c6_post</t>
+  </si>
+  <si>
+    <t>6554d5f1a5b42aea269aa82a_post</t>
+  </si>
+  <si>
+    <t>6533fca6a20c492a2baf878e_post</t>
+  </si>
+  <si>
+    <t>6510335c6c5ba95f95c5af89_post</t>
+  </si>
+  <si>
+    <t>654baf4c709dd68c04a8b09a_post</t>
+  </si>
+  <si>
+    <t>65674ca014879b38a634b741_post</t>
+  </si>
+  <si>
+    <t>65413d7a889c08941364abb6_post</t>
+  </si>
+  <si>
+    <t>6505b19314eb42b422d59509_post</t>
+  </si>
+  <si>
+    <t>653fbb7899638eb02212c25b_post</t>
+  </si>
+  <si>
+    <t>64e220abe394efe48bfe28f8_post</t>
+  </si>
+  <si>
+    <t>6557923d4a9cc0c7d81cd60d_post</t>
+  </si>
+  <si>
+    <t>607079a28a504f214dfd77b8_post</t>
+  </si>
+  <si>
+    <t>6503144bcc000df7879d9637_post</t>
+  </si>
+  <si>
+    <t>6543cbb6e554d07ea95a1db8_post</t>
+  </si>
+  <si>
+    <t>6517299ba3d7cde45394692a_post</t>
+  </si>
+  <si>
+    <t>644ac0e41a2fabcf5d563f20_post</t>
+  </si>
+  <si>
+    <t>6554d26c5dae0f7aa6a24b19_post</t>
+  </si>
+  <si>
+    <t>5fff0b0bcbc37a5f5928ed26_post</t>
+  </si>
+  <si>
+    <t>651311510abdac9c5b9c6c4b_post</t>
+  </si>
+  <si>
+    <t>615416df060f5730a1d4e113_post</t>
+  </si>
+  <si>
+    <t>656e5185676b397a22189d00_post</t>
+  </si>
+  <si>
+    <t>65410ad762a7e3c570b6273c_post</t>
+  </si>
+  <si>
+    <t>6516d284e2e240661699806c_post</t>
+  </si>
+  <si>
+    <t>64fdee2b969a06603ae3226d_post</t>
+  </si>
+  <si>
+    <t>5f738b981a302b0d6d6405aa_post</t>
+  </si>
+  <si>
+    <t>65465caa5dcdb76a16d563b3_post</t>
+  </si>
+  <si>
+    <t>5dea808cce8d8d19f5424b21_post</t>
+  </si>
+  <si>
+    <t>65170df8def70fb50be8068e_post</t>
+  </si>
+  <si>
+    <t>63c0157fbc63b6511d336764_post</t>
+  </si>
+  <si>
+    <t>615452aaabb932ada88ef3ca_post</t>
+  </si>
+  <si>
+    <t>5e6a3e3d265930022e81c70b_post</t>
+  </si>
+  <si>
+    <t>6524e0ef44178670528207b7_post</t>
+  </si>
+  <si>
+    <t>6572deb3c978dbcde1a8106c_post</t>
+  </si>
+  <si>
+    <t>6516d540a78298897619e273_post</t>
+  </si>
+  <si>
+    <t>651f003609736cc7a85d4328_post</t>
+  </si>
+  <si>
+    <t>653916355709faa03524b0df_post</t>
+  </si>
+  <si>
+    <t>638e2654a069e9c741d21ce3_post</t>
+  </si>
+  <si>
+    <t>65391c7ecf65866247606910_post</t>
+  </si>
+  <si>
+    <t>65674761184f5501367c963d_post</t>
+  </si>
+  <si>
+    <t>631f3fde43831da4ae27754b_post</t>
+  </si>
+  <si>
+    <t>63eb7c1abdbdf911ec1201ab_post</t>
+  </si>
+  <si>
+    <t>6518e333bba544ebf169f41b_post</t>
+  </si>
+  <si>
+    <t>650c02a928518783a1b963fd_post</t>
+  </si>
+  <si>
+    <t>5be95af71ca46b0001862746_post</t>
+  </si>
+  <si>
+    <t>5b0a869f1e55760001b93fa3_post</t>
+  </si>
+  <si>
+    <t>654b4a0e936bc8d3c57bfbf0_post</t>
+  </si>
+  <si>
+    <t>65182c5a0cadd3291661b9e0_post</t>
+  </si>
+  <si>
+    <t>6526a2a40ce1608344c552bc_post</t>
+  </si>
+  <si>
+    <t>5be454621effe60001cbf290_post</t>
+  </si>
+  <si>
+    <t>6529483ef2abe408d574860a_post</t>
+  </si>
+  <si>
+    <t>64ef6d994d6b1f11074bdfcf_post</t>
+  </si>
+  <si>
+    <t>5d43c606773d8b00016eaa8a_post</t>
+  </si>
+  <si>
+    <t>60fe7985ba99343ad0b893b7_post</t>
+  </si>
+  <si>
+    <t>60513ec07ee46769ed029be4_post</t>
+  </si>
+  <si>
+    <t>6516d4259c30f249ac643d4b_post</t>
+  </si>
+  <si>
+    <t>6516d321ac5a66a7aef87507_post</t>
+  </si>
+  <si>
+    <t>6565f2ba13586fa869dd3b28_post</t>
+  </si>
+  <si>
+    <t>63c54053d14cc248d3bffebd_post</t>
+  </si>
+  <si>
+    <t>650c42b04e90f6c176d20f48_post</t>
+  </si>
+  <si>
+    <t>611ba1976cd48fdde1f9edd3_post</t>
+  </si>
+  <si>
+    <t>59a426b35fd74b0001abfa4f_post</t>
+  </si>
+  <si>
+    <t>5bf4033ff719c9000153d38e_post</t>
+  </si>
+  <si>
+    <t>6480b160d51d051b42f67b3d_post</t>
+  </si>
+  <si>
+    <t>5aad4225811b2000016f6ed1_post</t>
+  </si>
+  <si>
+    <t>5e9f28299286a70a21369a87_post</t>
+  </si>
+  <si>
+    <t>655f017761462616d393ed61_post</t>
+  </si>
+  <si>
+    <t>6458f51ce9dfaceaf66923b7_post</t>
+  </si>
+  <si>
+    <t>6568ad4a9ad5cefdb6e70dc7_post</t>
+  </si>
+  <si>
+    <t>6516f474d21c67a9a5bbb712_post</t>
+  </si>
+  <si>
+    <t>604d17eb4931a500d6e0a3d3_post</t>
+  </si>
+  <si>
+    <t>655906b1346b2b209cd19772_post</t>
+  </si>
+  <si>
+    <t>64369636de5954c6029e89b4_post</t>
+  </si>
+  <si>
+    <t>6519d311acb10856b9cff800_post</t>
+  </si>
+  <si>
+    <t>6571d06ee2f60c04ca775e78_post</t>
+  </si>
+  <si>
+    <t>653671ae2ac8d502b52b1bb3_post</t>
+  </si>
+  <si>
+    <t>60fd15295d6b2a3711cafbd2_post</t>
+  </si>
+  <si>
+    <t>651758fd2a0e6965260a89fc_post</t>
+  </si>
+  <si>
+    <t>6427068bce4fc1aa335ad025_post</t>
+  </si>
+  <si>
+    <t>5dd08cf019eecb169dc131ba_post</t>
+  </si>
+  <si>
+    <t>627bbf69ab2788507bc421a2_post</t>
+  </si>
+  <si>
+    <t>5ebe6e4a226f3b1c53cd0626_post</t>
+  </si>
+  <si>
+    <t>63d02bd28e37a2abe1006c61_post</t>
+  </si>
+  <si>
+    <t>652d1a0830b934d1643b80c5_post</t>
+  </si>
+  <si>
+    <t>6517e9bc213462dc2254bd24_post</t>
+  </si>
+  <si>
+    <t>650ff7a187874a12d765b5ef_post</t>
+  </si>
+  <si>
+    <t>65170d2924df1aca5e1b075b_post</t>
+  </si>
+  <si>
+    <t>6517283ed2294dbc8561979d_post</t>
+  </si>
+  <si>
+    <t>65367487f0d1c1607d3665c9_post</t>
+  </si>
+  <si>
+    <t>654e379c8578beb912aee2ff_post</t>
+  </si>
+  <si>
+    <t>6039b30f86b21c537bfb9448_post</t>
+  </si>
+  <si>
+    <t>656c50a4c053d63a280ad6d0_post</t>
+  </si>
+  <si>
+    <t>6536973604f263f3c70495bf_post</t>
+  </si>
+  <si>
+    <t>654a45fc528885d395cd5cab_post</t>
+  </si>
+  <si>
+    <t>5c9fd46cfd19090012b4ac8b_post</t>
+  </si>
+  <si>
+    <t>646219bb0b91a6f3327e39fb_post</t>
+  </si>
+  <si>
+    <t>6384d76e3da4c98dc29e390b_post</t>
+  </si>
+  <si>
+    <t>6521569041baced19add37bc_post</t>
+  </si>
+  <si>
+    <t>5da727bfc2a70a0011a128e0_post</t>
+  </si>
+  <si>
+    <t>5de81f0edb424d7965702d2d_post</t>
+  </si>
+  <si>
+    <t>64f1e6cd05138cd766340792_post</t>
+  </si>
+  <si>
+    <t>64fee13e6324ea4884bcc9db_post</t>
+  </si>
+  <si>
+    <t>6505c50f48dfd793a7787b8a_post</t>
+  </si>
+  <si>
+    <t>63eb38339e72d01818aeb71b_post</t>
+  </si>
+  <si>
+    <t>65313217ba43953a5e06fcae_post</t>
+  </si>
+  <si>
+    <t>6571e455af2e5eae9adea54a_post</t>
+  </si>
+  <si>
+    <t>6123c4f8e486767a57db9afe_post</t>
+  </si>
+  <si>
+    <t>650c2a3e5ae50ab8668448de_post</t>
+  </si>
+  <si>
+    <t>653d060aaf01dfc1443ad299_post</t>
+  </si>
+  <si>
+    <t>650a5cc55e8ddf8bae0b81fb_post</t>
+  </si>
+  <si>
+    <t>640b7f3428d986ad3da9ebcf_post</t>
+  </si>
+  <si>
+    <t>653bb9c18fa69d049372d45f_post</t>
+  </si>
+  <si>
+    <t>5ed0f0bb34177d0009582f38_post</t>
+  </si>
+  <si>
+    <t>604d26915c5dc2a98d18c7fd_post</t>
+  </si>
+  <si>
+    <t>5dd5855018beb6544df7f797_post</t>
+  </si>
+  <si>
+    <t>63c33a62f56571779a295a6f_post</t>
+  </si>
+  <si>
+    <t>653bbdbd990bb0039d427925_post</t>
+  </si>
+  <si>
+    <t>5f298b2b7823df0a46e25d81_post</t>
+  </si>
+  <si>
+    <t>6559eb6c636ef499cb5e1f85_post</t>
+  </si>
+  <si>
+    <t>653be644c2d5f2b6d285699e_post</t>
+  </si>
+  <si>
+    <t>5edc8e2eaa0f2295a0fcef85_post</t>
+  </si>
+  <si>
+    <t>646b607e88557c2ff4f0de85_post</t>
+  </si>
+  <si>
+    <t>5fb42f807e81960acbfdb22e_post</t>
+  </si>
+  <si>
+    <t>62ed054b4bf00da20ea22dc2_post</t>
+  </si>
+  <si>
+    <t>629756625dc7cf458e36151f_post</t>
+  </si>
+  <si>
+    <t>650455b9cde6207c1ebd732b_post</t>
+  </si>
+  <si>
+    <t>603a80b01bb75f608c3dbb0d_post</t>
+  </si>
+  <si>
+    <t>65410b3f1de864e712bb267d_post</t>
+  </si>
+  <si>
+    <t>62c42b020ddc9564f77e2e24_post</t>
+  </si>
+  <si>
+    <t>6053d1011605ac6f3164bc99_post</t>
+  </si>
+  <si>
+    <t>65170641ac562bb61fb8e647_post</t>
+  </si>
+  <si>
+    <t>652680aaf06124cc46807a30_post</t>
+  </si>
+  <si>
+    <t>655b4ea3ab2c763e739cb199_post</t>
+  </si>
+  <si>
+    <t>6525ab791fb0b3aaf866d7c7_post</t>
+  </si>
+  <si>
+    <t>591a1f4800a5650001276188_post</t>
+  </si>
+  <si>
+    <t>655c754ee949a617a358b8c5_post</t>
+  </si>
+  <si>
+    <t>6304a2502fbdd7626ed9c2ac_post</t>
+  </si>
+  <si>
+    <t>652fe4a08d5ecae18fc4fe31_post</t>
+  </si>
+  <si>
+    <t>6543aeb6dd91d965fc3df508_post</t>
+  </si>
+  <si>
+    <t>6536b3467fc9c8f7dbabcf51_post</t>
+  </si>
+  <si>
+    <t>653d07d22dd9d12c6e7b8082_post</t>
+  </si>
+  <si>
+    <t>6538ef6ac2e74e7d85a136ca_post</t>
+  </si>
+  <si>
+    <t>63b6be975097f6e31872fc0e_post</t>
+  </si>
+  <si>
+    <t>6544ea06d33e1704f993f76f_post</t>
+  </si>
+  <si>
+    <t>60207652caa62b6a34ff96dc_post</t>
+  </si>
+  <si>
+    <t>610905a730569ffea2fbdd0b_post</t>
+  </si>
+  <si>
+    <t>5a942689b5e2110001c67d93_post</t>
+  </si>
+  <si>
+    <t>645b8b2128bbb68d29778068_post</t>
+  </si>
+  <si>
+    <t>6516d3c10cc8996984d514f4_post</t>
+  </si>
+  <si>
+    <t>604b169fe4b7991ec08da3a6_post</t>
+  </si>
+  <si>
+    <t>6569ffc2439eb88f22d4e8bc_post</t>
+  </si>
+  <si>
+    <t>5fcf9f17f5a7c20ba38e9cc9_post</t>
+  </si>
+  <si>
+    <t>64ff13ded28d546281ffb6b5_post</t>
+  </si>
+  <si>
+    <t>6544fd5d0fb2eaaf83e2ddc9_post</t>
+  </si>
+  <si>
+    <t>63fd0b137e38c72ea19176aa_post</t>
+  </si>
+  <si>
+    <t>653a50254cd0995ce9fed45e_post</t>
+  </si>
+  <si>
+    <t>651ec655d2ef1a3ba8e64470_post</t>
+  </si>
+  <si>
+    <t>5a7fab56f49c9a0001f3549e_post</t>
+  </si>
+  <si>
+    <t>6554d1f1fda70c02063f51bd_post</t>
+  </si>
+  <si>
+    <t>6552628d0dfe6b458c390708_post</t>
+  </si>
+  <si>
+    <t>5b21646bdf28a7000166f4dc_post</t>
+  </si>
+  <si>
+    <t>6568ccd0468b7384e18af74b_post</t>
+  </si>
+  <si>
+    <t>6480b08b4e783b4c327cf4a8_post</t>
+  </si>
+  <si>
+    <t>6505e770a24e4561f219381e_post</t>
+  </si>
+  <si>
+    <t>653adf50c2b4d95715fa0383_post</t>
+  </si>
+  <si>
+    <t>63dfd4fb58435f30c7e5b04b_post</t>
+  </si>
+  <si>
+    <t>65526268c396c0c75dcefdf2_post</t>
+  </si>
+  <si>
+    <t>6560c1ff0b97f1d037b3c2dd_post</t>
+  </si>
+  <si>
+    <t>6521ac4e830108f7281e8644_post</t>
+  </si>
+  <si>
+    <t>606b94352e103bc54d43321b_post</t>
+  </si>
+  <si>
+    <t>64e74f0c7ba1863371602661_post</t>
+  </si>
+  <si>
+    <t>6532825749ca31d35c5cc482_post</t>
+  </si>
+  <si>
+    <t>63b87d2c9edd47ad702413a1_post</t>
+  </si>
+  <si>
+    <t>5f32d5f107d49607c3f6cf7a_post</t>
+  </si>
+  <si>
+    <t>6429682ff18d08f9eed7d9e7_post</t>
+  </si>
+  <si>
+    <t>643c243ff0ef4cb25c20a392_post</t>
+  </si>
+  <si>
+    <t>63cf5dcd6dbd0452632b58bb_post</t>
+  </si>
+  <si>
+    <t>617082143afa2b9f049f8b3b_post</t>
+  </si>
+  <si>
+    <t>647e2500ac34cb60b8e1348d_post</t>
+  </si>
+  <si>
+    <t>61574c44d4bd510e680f9d7a_post</t>
+  </si>
+  <si>
+    <t>6516ff4cda6f1e36fd05b1cc_post</t>
+  </si>
+  <si>
+    <t>5f4cde1cbfcaa81fc4dbf57d_post</t>
+  </si>
+  <si>
+    <t>6561ff666e87c03638f8fb11_post</t>
+  </si>
+  <si>
+    <t>64539733186ad1764e4c2b74_post</t>
+  </si>
+  <si>
+    <t>63cfbea470ab1bba9db30082_post</t>
+  </si>
+  <si>
+    <t>65034478b7a228b2bdfdca5c_post</t>
+  </si>
+  <si>
+    <t>6526b4db08c36959a00e69c4_post</t>
+  </si>
+  <si>
+    <t>6537d0d238ce085ea079c318_post</t>
+  </si>
+  <si>
+    <t>6570908f385d595d5df25c68_post</t>
+  </si>
+  <si>
+    <t>652156df21a8be7bb4c6f4e7_post</t>
+  </si>
+  <si>
+    <t>616b2d4ff5ffb8b86c08661b_post</t>
+  </si>
+  <si>
+    <t>65426792dac360c44e4908a7_post</t>
+  </si>
+  <si>
+    <t>65772f25af9bdd7c3ae47af5_post</t>
+  </si>
+  <si>
+    <t>652d2a7b11d97787933195c6_post</t>
+  </si>
+  <si>
+    <t>6516d85620c0017a8db27afc_post</t>
+  </si>
+  <si>
+    <t>654a76de0874380f590ca432_post</t>
+  </si>
+  <si>
+    <t>63eb514012c203a7a2146262_post</t>
+  </si>
+  <si>
+    <t>6046b9bf731b0611fe4d0159_post</t>
+  </si>
+  <si>
+    <t>5f5494aa76d6147f7ca89533_post</t>
+  </si>
+  <si>
+    <t>5e5fbff6de7bcc2fc7f396db_post</t>
+  </si>
+  <si>
+    <t>613b5e02f007dc6d30164fb3_post</t>
+  </si>
+  <si>
+    <t>64f1e17e5439f81a8eade6c2_post</t>
+  </si>
+  <si>
+    <t>5bceffb6a69cc50001d42ea5_post</t>
+  </si>
+  <si>
+    <t>60fd19bb0d1f1d54adccc4fa_post</t>
   </si>
 </sst>
 </file>
@@ -2305,7 +2305,7 @@
         <v>0.6550570641479733</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7423890598447433</v>
+        <v>0.7423890598447432</v>
       </c>
       <c r="L2" t="n">
         <v>2.375</v>
@@ -2359,7 +2359,7 @@
         <v>0.3167701863354033</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.5125651967757228</v>
+        <v>-0.5125651967757225</v>
       </c>
       <c r="AD2"/>
       <c r="AE2" t="n">
@@ -2563,7 +2563,7 @@
         <v>0.38667929292929293</v>
       </c>
       <c r="K4" t="n">
-        <v>0.5414506112685872</v>
+        <v>0.5414506112685873</v>
       </c>
       <c r="L4" t="n">
         <v>5.5</v>
@@ -2617,7 +2617,7 @@
         <v>0.6161616161616164</v>
       </c>
       <c r="AC4" t="n">
-        <v>-0.6285714285714293</v>
+        <v>-0.6285714285714283</v>
       </c>
       <c r="AD4"/>
       <c r="AE4" t="n">
@@ -2692,7 +2692,7 @@
         <v>0.35174603174603175</v>
       </c>
       <c r="K5" t="n">
-        <v>0.7400106338867257</v>
+        <v>0.7400106338867255</v>
       </c>
       <c r="L5" t="n">
         <v>1.8</v>
@@ -2875,7 +2875,7 @@
         <v>-0.83448275862069</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.9929119905493207</v>
+        <v>-0.9929119905493199</v>
       </c>
       <c r="AD6" t="n">
         <v>2.0</v>
@@ -2950,7 +2950,7 @@
         <v>0.6640576230492197</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8196150948842338</v>
+        <v>0.8196150948842342</v>
       </c>
       <c r="L7" t="n">
         <v>2.706896551724138</v>
@@ -3004,7 +3004,7 @@
         <v>0.6376988984088133</v>
       </c>
       <c r="AC7" t="n">
-        <v>-0.30237489397794753</v>
+        <v>-0.30237489397794787</v>
       </c>
       <c r="AD7"/>
       <c r="AE7" t="n">
@@ -3133,7 +3133,7 @@
         <v>0.3708737864077671</v>
       </c>
       <c r="AC8" t="n">
-        <v>-0.2404287901990813</v>
+        <v>-0.24042879019908114</v>
       </c>
       <c r="AD8"/>
       <c r="AE8" t="n">
@@ -3208,7 +3208,7 @@
         <v>0.5971354166666667</v>
       </c>
       <c r="K9" t="n">
-        <v>0.677944701022678</v>
+        <v>0.6779447010226782</v>
       </c>
       <c r="L9" t="n">
         <v>1.6829268292682926</v>
@@ -3262,7 +3262,7 @@
         <v>0.1809317443120259</v>
       </c>
       <c r="AC9" t="n">
-        <v>-0.5842547545333925</v>
+        <v>-0.5842547545333923</v>
       </c>
       <c r="AD9"/>
       <c r="AE9" t="n">
@@ -3337,7 +3337,7 @@
         <v>0.8091005291005292</v>
       </c>
       <c r="K10" t="n">
-        <v>0.7414111553854236</v>
+        <v>0.7414111553854239</v>
       </c>
       <c r="L10" t="n">
         <v>3.576</v>
@@ -3391,7 +3391,7 @@
         <v>0.14006514657980465</v>
       </c>
       <c r="AC10" t="n">
-        <v>-0.390251021599533</v>
+        <v>-0.3902510215995334</v>
       </c>
       <c r="AD10"/>
       <c r="AE10" t="n">
@@ -3466,7 +3466,7 @@
         <v>0.615625</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7300163799033653</v>
+        <v>0.7300163799033658</v>
       </c>
       <c r="L11" t="n">
         <v>1.8181818181818181</v>
@@ -3649,7 +3649,7 @@
         <v>-0.34847298355520734</v>
       </c>
       <c r="AC12" t="n">
-        <v>-0.21293103448275805</v>
+        <v>-0.2129310344827581</v>
       </c>
       <c r="AD12" t="n">
         <v>2.0</v>
@@ -3724,7 +3724,7 @@
         <v>0.6273015873015872</v>
       </c>
       <c r="K13" t="n">
-        <v>0.7296017761127144</v>
+        <v>0.7296017761127148</v>
       </c>
       <c r="L13" t="n">
         <v>3.375</v>
@@ -3778,7 +3778,7 @@
         <v>-0.2315270935960584</v>
       </c>
       <c r="AC13" t="n">
-        <v>-0.7738791423001952</v>
+        <v>-0.773879142300195</v>
       </c>
       <c r="AD13"/>
       <c r="AE13" t="n">
@@ -3853,7 +3853,7 @@
         <v>0.645079365079365</v>
       </c>
       <c r="K14" t="n">
-        <v>0.6778002862471614</v>
+        <v>0.6778002862471612</v>
       </c>
       <c r="L14" t="n">
         <v>2.8947368421052633</v>
@@ -3907,7 +3907,7 @@
         <v>0.885714285714286</v>
       </c>
       <c r="AC14" t="n">
-        <v>-0.7224880382775118</v>
+        <v>-0.7224880382775122</v>
       </c>
       <c r="AD14"/>
       <c r="AE14" t="n">
@@ -3982,7 +3982,7 @@
         <v>0.5733333333333334</v>
       </c>
       <c r="K15" t="n">
-        <v>0.7205526401883152</v>
+        <v>0.720552640188315</v>
       </c>
       <c r="L15" t="n">
         <v>2.303030303030303</v>
@@ -4111,7 +4111,7 @@
         <v>0.4965504720406681</v>
       </c>
       <c r="K16" t="n">
-        <v>0.7738283863607281</v>
+        <v>0.7738283863607275</v>
       </c>
       <c r="L16" t="n">
         <v>1.8048780487804879</v>
@@ -4165,7 +4165,7 @@
         <v>0.19941348973607007</v>
       </c>
       <c r="AC16" t="n">
-        <v>-0.26126126126126126</v>
+        <v>-0.2612612612612614</v>
       </c>
       <c r="AD16"/>
       <c r="AE16" t="n">
@@ -4240,7 +4240,7 @@
         <v>0.6711111111111111</v>
       </c>
       <c r="K17" t="n">
-        <v>0.7291671489030337</v>
+        <v>0.7291671489030339</v>
       </c>
       <c r="L17" t="n">
         <v>3.0</v>
@@ -4294,7 +4294,7 @@
         <v>-0.5525114155251146</v>
       </c>
       <c r="AC17" t="n">
-        <v>-0.8859649122807021</v>
+        <v>-0.8859649122807024</v>
       </c>
       <c r="AD17"/>
       <c r="AE17" t="n">
@@ -4369,7 +4369,7 @@
         <v>0.42140039447731764</v>
       </c>
       <c r="K18" t="n">
-        <v>0.5849811521556811</v>
+        <v>0.5849811521556812</v>
       </c>
       <c r="L18" t="n">
         <v>2.25</v>
@@ -4423,7 +4423,7 @@
         <v>0.020942408376963276</v>
       </c>
       <c r="AC18" t="n">
-        <v>-0.2222222222222223</v>
+        <v>-0.22222222222222215</v>
       </c>
       <c r="AD18"/>
       <c r="AE18" t="n">
@@ -4498,7 +4498,7 @@
         <v>0.596646942800789</v>
       </c>
       <c r="K19" t="n">
-        <v>0.7217444379347059</v>
+        <v>0.7217444379347061</v>
       </c>
       <c r="L19" t="n">
         <v>1.434782608695652</v>
@@ -4627,7 +4627,7 @@
         <v>0.6805555555555556</v>
       </c>
       <c r="K20" t="n">
-        <v>0.7503994041344022</v>
+        <v>0.7503994041344021</v>
       </c>
       <c r="L20" t="n">
         <v>1.5</v>
@@ -4681,7 +4681,7 @@
         <v>-0.615384615384616</v>
       </c>
       <c r="AC20" t="n">
-        <v>-0.9224489795918367</v>
+        <v>-0.9224489795918362</v>
       </c>
       <c r="AD20" t="n">
         <v>2.0</v>
@@ -4756,7 +4756,7 @@
         <v>0.375</v>
       </c>
       <c r="K21" t="n">
-        <v>0.5302559999458111</v>
+        <v>0.530255999945811</v>
       </c>
       <c r="L21" t="n">
         <v>1.7435897435897436</v>
@@ -4810,7 +4810,7 @@
         <v>-0.34615384615384664</v>
       </c>
       <c r="AC21" t="n">
-        <v>-0.7342799188640976</v>
+        <v>-0.7342799188640978</v>
       </c>
       <c r="AD21"/>
       <c r="AE21" t="n">
@@ -4939,7 +4939,7 @@
         <v>0.4958448753462602</v>
       </c>
       <c r="AC22" t="n">
-        <v>-0.9753381066030233</v>
+        <v>-0.9753381066030232</v>
       </c>
       <c r="AD22"/>
       <c r="AE22" t="n">
@@ -5014,7 +5014,7 @@
         <v>0.6279365079365079</v>
       </c>
       <c r="K23" t="n">
-        <v>0.7074750507941108</v>
+        <v>0.7074750507941109</v>
       </c>
       <c r="L23" t="n">
         <v>1.8461538461538463</v>
@@ -5143,7 +5143,7 @@
         <v>0.44635416666666666</v>
       </c>
       <c r="K24" t="n">
-        <v>0.6515685568801917</v>
+        <v>0.6515685568801912</v>
       </c>
       <c r="L24" t="n">
         <v>3.1587301587301586</v>
@@ -5197,7 +5197,7 @@
         <v>-0.004566210045662004</v>
       </c>
       <c r="AC24" t="n">
-        <v>-0.41538461538461546</v>
+        <v>-0.4153846153846151</v>
       </c>
       <c r="AD24"/>
       <c r="AE24" t="n">
@@ -5272,7 +5272,7 @@
         <v>0.5149136577708007</v>
       </c>
       <c r="K25" t="n">
-        <v>0.7202576681922632</v>
+        <v>0.7202576681922627</v>
       </c>
       <c r="L25" t="n">
         <v>2.1372549019607843</v>
@@ -5401,7 +5401,7 @@
         <v>0.6214876033057851</v>
       </c>
       <c r="K26" t="n">
-        <v>0.6848446400614066</v>
+        <v>0.6848446400614067</v>
       </c>
       <c r="L26" t="n">
         <v>2.5294117647058822</v>
@@ -5455,7 +5455,7 @@
         <v>-0.5014836795252229</v>
       </c>
       <c r="AC26" t="n">
-        <v>-0.9616666666666671</v>
+        <v>-0.9616666666666669</v>
       </c>
       <c r="AD26"/>
       <c r="AE26" t="n">
@@ -5530,7 +5530,7 @@
         <v>0.633256704980843</v>
       </c>
       <c r="K27" t="n">
-        <v>0.7808668713731202</v>
+        <v>0.7808668713731198</v>
       </c>
       <c r="L27" t="n">
         <v>1.6</v>
@@ -5584,7 +5584,7 @@
         <v>0.2169491525423726</v>
       </c>
       <c r="AC27" t="n">
-        <v>-0.39465506525792377</v>
+        <v>-0.3946550652579232</v>
       </c>
       <c r="AD27" t="n">
         <v>2.0</v>
@@ -5659,7 +5659,7 @@
         <v>0.5514705882352942</v>
       </c>
       <c r="K28" t="n">
-        <v>0.7020627893552882</v>
+        <v>0.702062789355288</v>
       </c>
       <c r="L28" t="n">
         <v>2.89010989010989</v>
@@ -5788,7 +5788,7 @@
         <v>0.6534090909090909</v>
       </c>
       <c r="K29" t="n">
-        <v>0.6931124125449201</v>
+        <v>0.69311241254492</v>
       </c>
       <c r="L29" t="n">
         <v>1.375</v>
@@ -5842,7 +5842,7 @@
         <v>-0.35578947368420966</v>
       </c>
       <c r="AC29" t="n">
-        <v>-0.7868538608806641</v>
+        <v>-0.7868538608806628</v>
       </c>
       <c r="AD29"/>
       <c r="AE29" t="n">
@@ -5917,7 +5917,7 @@
         <v>0.592</v>
       </c>
       <c r="K30" t="n">
-        <v>0.8015047946529142</v>
+        <v>0.801504794652914</v>
       </c>
       <c r="L30" t="n">
         <v>2.5057471264367814</v>
@@ -6046,7 +6046,7 @@
         <v>0.546031746031746</v>
       </c>
       <c r="K31" t="n">
-        <v>0.677040595518613</v>
+        <v>0.6770405955186132</v>
       </c>
       <c r="L31" t="n">
         <v>2.6</v>
@@ -6175,7 +6175,7 @@
         <v>0.51010101010101</v>
       </c>
       <c r="K32" t="n">
-        <v>0.6221522568492123</v>
+        <v>0.6221522568492124</v>
       </c>
       <c r="L32" t="n">
         <v>1.6538461538461537</v>
@@ -6229,7 +6229,7 @@
         <v>-0.3333333333333335</v>
       </c>
       <c r="AC32" t="n">
-        <v>-0.6853932584269661</v>
+        <v>-0.685393258426967</v>
       </c>
       <c r="AD32" t="n">
         <v>3.0</v>
@@ -6304,7 +6304,7 @@
         <v>0.606943125461644</v>
       </c>
       <c r="K33" t="n">
-        <v>0.791112308703898</v>
+        <v>0.7911123087038979</v>
       </c>
       <c r="L33" t="n">
         <v>2.1717171717171717</v>
@@ -6487,7 +6487,7 @@
         <v>-0.007194244604314907</v>
       </c>
       <c r="AC34" t="n">
-        <v>-0.291946308724832</v>
+        <v>-0.291946308724831</v>
       </c>
       <c r="AD34"/>
       <c r="AE34" t="n">
@@ -6562,7 +6562,7 @@
         <v>0.6302636757182212</v>
       </c>
       <c r="K35" t="n">
-        <v>0.7056051838996015</v>
+        <v>0.705605183899602</v>
       </c>
       <c r="L35" t="n">
         <v>3.45</v>
@@ -6616,7 +6616,7 @@
         <v>0.18518518518518515</v>
       </c>
       <c r="AC35" t="n">
-        <v>-0.37647058823529417</v>
+        <v>-0.37647058823529406</v>
       </c>
       <c r="AD35"/>
       <c r="AE35" t="n">
@@ -6691,7 +6691,7 @@
         <v>0.5707166179755971</v>
       </c>
       <c r="K36" t="n">
-        <v>0.770607464020739</v>
+        <v>0.7706074640207358</v>
       </c>
       <c r="L36" t="n">
         <v>1.7878787878787878</v>
@@ -6745,7 +6745,7 @@
         <v>0.39964264443120867</v>
       </c>
       <c r="AC36" t="n">
-        <v>-0.861880133860663</v>
+        <v>-0.8618801338606629</v>
       </c>
       <c r="AD36"/>
       <c r="AE36" t="n">
@@ -6820,7 +6820,7 @@
         <v>0.4991349480968858</v>
       </c>
       <c r="K37" t="n">
-        <v>0.6972540736554399</v>
+        <v>0.6972540736554398</v>
       </c>
       <c r="L37" t="n">
         <v>1.9230769230769231</v>
@@ -6874,7 +6874,7 @@
         <v>-0.15076923076922957</v>
       </c>
       <c r="AC37" t="n">
-        <v>-0.4945054945054943</v>
+        <v>-0.494505494505495</v>
       </c>
       <c r="AD37"/>
       <c r="AE37" t="n">
@@ -6949,7 +6949,7 @@
         <v>0.595679012345679</v>
       </c>
       <c r="K38" t="n">
-        <v>0.6536855299290218</v>
+        <v>0.6536855299290221</v>
       </c>
       <c r="L38" t="n">
         <v>1.3333333333333333</v>
@@ -7003,7 +7003,7 @@
         <v>-0.547511312217195</v>
       </c>
       <c r="AC38" t="n">
-        <v>-0.9338842975206612</v>
+        <v>-0.9338842975206609</v>
       </c>
       <c r="AD38" t="n">
         <v>2.0</v>
@@ -7078,7 +7078,7 @@
         <v>0.6279365079365079</v>
       </c>
       <c r="K39" t="n">
-        <v>0.6750867163585549</v>
+        <v>0.6750867163585544</v>
       </c>
       <c r="L39" t="n">
         <v>3.8625</v>
@@ -7132,7 +7132,7 @@
         <v>-0.15151515151515182</v>
       </c>
       <c r="AC39" t="n">
-        <v>-0.47572815533980567</v>
+        <v>-0.4757281553398062</v>
       </c>
       <c r="AD39"/>
       <c r="AE39" t="n">
@@ -7207,7 +7207,7 @@
         <v>0.6043956043956044</v>
       </c>
       <c r="K40" t="n">
-        <v>0.6192501947457051</v>
+        <v>0.6192501947457056</v>
       </c>
       <c r="L40" t="n">
         <v>2.875</v>
@@ -7261,7 +7261,7 @@
         <v>-0.5423728813559318</v>
       </c>
       <c r="AC40" t="n">
-        <v>-0.9929119905493207</v>
+        <v>-0.9929119905493199</v>
       </c>
       <c r="AD40"/>
       <c r="AE40" t="n">
@@ -7336,7 +7336,7 @@
         <v>0.6056</v>
       </c>
       <c r="K41" t="n">
-        <v>0.7263578664227305</v>
+        <v>0.7263578664227307</v>
       </c>
       <c r="L41" t="n">
         <v>1.8409090909090908</v>
@@ -7390,7 +7390,7 @@
         <v>0.5770234986945174</v>
       </c>
       <c r="AC41" t="n">
-        <v>-0.16793893129770984</v>
+        <v>-0.16793893129770948</v>
       </c>
       <c r="AD41"/>
       <c r="AE41" t="n">
@@ -7465,7 +7465,7 @@
         <v>0.6429752066115703</v>
       </c>
       <c r="K42" t="n">
-        <v>0.7355499095234124</v>
+        <v>0.735549909523412</v>
       </c>
       <c r="L42" t="n">
         <v>2.3333333333333335</v>
@@ -7519,7 +7519,7 @@
         <v>-0.010204081632653862</v>
       </c>
       <c r="AC42" t="n">
-        <v>-0.432950191570881</v>
+        <v>-0.43295019157088077</v>
       </c>
       <c r="AD42"/>
       <c r="AE42" t="n">
@@ -7648,7 +7648,7 @@
         <v>-0.013793103448275425</v>
       </c>
       <c r="AC43" t="n">
-        <v>-0.3301343570057584</v>
+        <v>-0.3301343570057569</v>
       </c>
       <c r="AD43" t="n">
         <v>4.0</v>
@@ -7777,7 +7777,7 @@
         <v>0.37172774869109887</v>
       </c>
       <c r="AC44" t="n">
-        <v>-0.7113043478260872</v>
+        <v>-0.711304347826087</v>
       </c>
       <c r="AD44"/>
       <c r="AE44" t="n">
@@ -7852,7 +7852,7 @@
         <v>0.6370808678500987</v>
       </c>
       <c r="K45" t="n">
-        <v>0.6621504322623794</v>
+        <v>0.6621504322623792</v>
       </c>
       <c r="L45" t="n">
         <v>3.533333333333333</v>
@@ -7906,7 +7906,7 @@
         <v>-0.3071638861629047</v>
       </c>
       <c r="AC45" t="n">
-        <v>-0.6784565916398712</v>
+        <v>-0.6784565916398705</v>
       </c>
       <c r="AD45"/>
       <c r="AE45" t="n">
@@ -7981,7 +7981,7 @@
         <v>0.6400394477317555</v>
       </c>
       <c r="K46" t="n">
-        <v>0.7085243743539138</v>
+        <v>0.7085243743539129</v>
       </c>
       <c r="L46" t="n">
         <v>1.8333333333333333</v>
@@ -8035,7 +8035,7 @@
         <v>-0.6095238095238099</v>
       </c>
       <c r="AC46" t="n">
-        <v>-0.9753381066030233</v>
+        <v>-0.9753381066030232</v>
       </c>
       <c r="AD46" t="n">
         <v>2.0</v>
@@ -8110,7 +8110,7 @@
         <v>0.6699346405228758</v>
       </c>
       <c r="K47" t="n">
-        <v>0.7122802625711889</v>
+        <v>0.712280262571189</v>
       </c>
       <c r="L47" t="n">
         <v>1.3793103448275863</v>
@@ -8164,7 +8164,7 @@
         <v>-0.2941176470588234</v>
       </c>
       <c r="AC47" t="n">
-        <v>-0.4746621621621623</v>
+        <v>-0.47466216216216217</v>
       </c>
       <c r="AD47"/>
       <c r="AE47" t="n">
@@ -8239,7 +8239,7 @@
         <v>0.5072916666666667</v>
       </c>
       <c r="K48" t="n">
-        <v>0.6410418120233884</v>
+        <v>0.6410418120233881</v>
       </c>
       <c r="L48" t="n">
         <v>3.051282051282051</v>
@@ -8293,7 +8293,7 @@
         <v>0.18940397350993482</v>
       </c>
       <c r="AC48" t="n">
-        <v>-0.6326530612244899</v>
+        <v>-0.6326530612244902</v>
       </c>
       <c r="AD48"/>
       <c r="AE48" t="n">
@@ -8368,7 +8368,7 @@
         <v>0.5542406311637081</v>
       </c>
       <c r="K49" t="n">
-        <v>0.5814868443938437</v>
+        <v>0.5814868443938438</v>
       </c>
       <c r="L49" t="n">
         <v>2.6666666666666665</v>
@@ -8497,7 +8497,7 @@
         <v>0.5795454545454546</v>
       </c>
       <c r="K50" t="n">
-        <v>0.5876751203535706</v>
+        <v>0.5876751203535705</v>
       </c>
       <c r="L50" t="n">
         <v>2.7142857142857144</v>
@@ -8551,7 +8551,7 @@
         <v>-0.6000000000000001</v>
       </c>
       <c r="AC50" t="n">
-        <v>-0.9882491186839014</v>
+        <v>-0.9882491186839015</v>
       </c>
       <c r="AD50"/>
       <c r="AE50" t="n">
@@ -8626,7 +8626,7 @@
         <v>0.3952020202020202</v>
       </c>
       <c r="K51" t="n">
-        <v>0.6741270607693663</v>
+        <v>0.6741270607693659</v>
       </c>
       <c r="L51" t="n">
         <v>2.840909090909091</v>
@@ -8680,7 +8680,7 @@
         <v>0.05691056910569063</v>
       </c>
       <c r="AC51" t="n">
-        <v>-0.48429319371727647</v>
+        <v>-0.484293193717277</v>
       </c>
       <c r="AD51"/>
       <c r="AE51" t="n">
@@ -8755,7 +8755,7 @@
         <v>0.47672583826429976</v>
       </c>
       <c r="K52" t="n">
-        <v>0.5923475419384225</v>
+        <v>0.5923475419384224</v>
       </c>
       <c r="L52" t="n">
         <v>2.8679245283018866</v>
@@ -8809,7 +8809,7 @@
         <v>-0.12365591397849367</v>
       </c>
       <c r="AC52" t="n">
-        <v>-0.6656546489563565</v>
+        <v>-0.6656546489563578</v>
       </c>
       <c r="AD52" t="n">
         <v>2.0</v>
@@ -8884,7 +8884,7 @@
         <v>0.5047428542673108</v>
       </c>
       <c r="K53" t="n">
-        <v>0.7556211655864186</v>
+        <v>0.7556211655864188</v>
       </c>
       <c r="L53" t="n">
         <v>3.2181818181818183</v>
@@ -8938,7 +8938,7 @@
         <v>0.1630791681867943</v>
       </c>
       <c r="AC53" t="n">
-        <v>-0.32379484921857804</v>
+        <v>-0.32379484921857793</v>
       </c>
       <c r="AD53"/>
       <c r="AE53" t="n">
@@ -9067,7 +9067,7 @@
         <v>-0.615384615384616</v>
       </c>
       <c r="AC54" t="n">
-        <v>-0.9224489795918367</v>
+        <v>-0.9224489795918362</v>
       </c>
       <c r="AD54" t="n">
         <v>2.0</v>
@@ -9142,7 +9142,7 @@
         <v>0.17851239669421487</v>
       </c>
       <c r="K55" t="n">
-        <v>0.503426796616737</v>
+        <v>0.5034267966167372</v>
       </c>
       <c r="L55" t="n">
         <v>3.185185185185185</v>
@@ -9196,7 +9196,7 @@
         <v>0.09396914446002946</v>
       </c>
       <c r="AC55" t="n">
-        <v>-0.0897435897435898</v>
+        <v>-0.0897435897435909</v>
       </c>
       <c r="AD55"/>
       <c r="AE55" t="n">
@@ -9271,7 +9271,7 @@
         <v>0.48444444444444446</v>
       </c>
       <c r="K56" t="n">
-        <v>0.5361560968173988</v>
+        <v>0.5361560968173986</v>
       </c>
       <c r="L56" t="n">
         <v>4.0</v>
@@ -9325,7 +9325,7 @@
         <v>-0.09090909090909091</v>
       </c>
       <c r="AC56" t="n">
-        <v>-0.6363636363636365</v>
+        <v>-0.6363636363636361</v>
       </c>
       <c r="AD56"/>
       <c r="AE56" t="n">
@@ -9400,7 +9400,7 @@
         <v>0.3371271585557299</v>
       </c>
       <c r="K57" t="n">
-        <v>0.6461823403930269</v>
+        <v>0.6461823403930266</v>
       </c>
       <c r="L57" t="n">
         <v>2.2954545454545454</v>
@@ -9454,7 +9454,7 @@
         <v>-0.17614804660726485</v>
       </c>
       <c r="AC57" t="n">
-        <v>-0.6379440665154948</v>
+        <v>-0.6379440665154945</v>
       </c>
       <c r="AD57" t="n">
         <v>4.0</v>
@@ -9529,7 +9529,7 @@
         <v>0.5601577909270217</v>
       </c>
       <c r="K58" t="n">
-        <v>0.651744874255984</v>
+        <v>0.6517448742559838</v>
       </c>
       <c r="L58" t="n">
         <v>2.1025641025641026</v>
@@ -9583,7 +9583,7 @@
         <v>0.22580645161290333</v>
       </c>
       <c r="AC58" t="n">
-        <v>-0.718108831400535</v>
+        <v>-0.7181088314005353</v>
       </c>
       <c r="AD58"/>
       <c r="AE58" t="n">
@@ -9658,7 +9658,7 @@
         <v>0.5444444444444444</v>
       </c>
       <c r="K59" t="n">
-        <v>0.5463907883734855</v>
+        <v>0.5463907883734856</v>
       </c>
       <c r="L59" t="n">
         <v>2.6666666666666665</v>
@@ -9712,7 +9712,7 @@
         <v>-0.5625000000000008</v>
       </c>
       <c r="AC59" t="n">
-        <v>-0.9783197831978322</v>
+        <v>-0.9783197831978324</v>
       </c>
       <c r="AD59"/>
       <c r="AE59" t="n">
@@ -9787,7 +9787,7 @@
         <v>0.6400394477317555</v>
       </c>
       <c r="K60" t="n">
-        <v>0.7085243743539135</v>
+        <v>0.7085243743539137</v>
       </c>
       <c r="L60" t="n">
         <v>2.8484848484848486</v>
@@ -9841,7 +9841,7 @@
         <v>-0.6095238095238099</v>
       </c>
       <c r="AC60" t="n">
-        <v>-0.9753381066030233</v>
+        <v>-0.9753381066030232</v>
       </c>
       <c r="AD60"/>
       <c r="AE60" t="n">
@@ -10045,7 +10045,7 @@
         <v>0.44232804232804224</v>
       </c>
       <c r="K62" t="n">
-        <v>0.712617024991619</v>
+        <v>0.7126170249916194</v>
       </c>
       <c r="L62" t="n">
         <v>2.5416666666666665</v>
@@ -10174,7 +10174,7 @@
         <v>0.542386185243328</v>
       </c>
       <c r="K63" t="n">
-        <v>0.6797318422492199</v>
+        <v>0.6797318422492201</v>
       </c>
       <c r="L63" t="n">
         <v>1.82</v>
@@ -10303,7 +10303,7 @@
         <v>0.34201058201058204</v>
       </c>
       <c r="K64" t="n">
-        <v>0.5581775385070359</v>
+        <v>0.5581775385070363</v>
       </c>
       <c r="L64" t="n">
         <v>1.9811320754716981</v>
@@ -10357,7 +10357,7 @@
         <v>0.16317991631799184</v>
       </c>
       <c r="AC64" t="n">
-        <v>-0.5340086830680171</v>
+        <v>-0.5340086830680167</v>
       </c>
       <c r="AD64" t="n">
         <v>3.0</v>
@@ -10432,7 +10432,7 @@
         <v>0.6805555555555556</v>
       </c>
       <c r="K65" t="n">
-        <v>0.7503994041344021</v>
+        <v>0.7503994041344023</v>
       </c>
       <c r="L65" t="n">
         <v>1.9166666666666667</v>
@@ -10486,7 +10486,7 @@
         <v>0.8321678321678306</v>
       </c>
       <c r="AC65" t="n">
-        <v>-0.9224489795918367</v>
+        <v>-0.9224489795918362</v>
       </c>
       <c r="AD65"/>
       <c r="AE65" t="n">
@@ -10615,7 +10615,7 @@
         <v>-0.40663176265270523</v>
       </c>
       <c r="AC66" t="n">
-        <v>-0.71900826446281</v>
+        <v>-0.7190082644628101</v>
       </c>
       <c r="AD66"/>
       <c r="AE66" t="n">
@@ -10690,7 +10690,7 @@
         <v>0.487889979248004</v>
       </c>
       <c r="K67" t="n">
-        <v>0.6177896110867338</v>
+        <v>0.617789611086734</v>
       </c>
       <c r="L67" t="n">
         <v>5.133333333333334</v>
@@ -10744,7 +10744,7 @@
         <v>0.4819494584837544</v>
       </c>
       <c r="AC67" t="n">
-        <v>-0.43613633683217407</v>
+        <v>-0.4361363368321737</v>
       </c>
       <c r="AD67"/>
       <c r="AE67" t="n">
@@ -10819,7 +10819,7 @@
         <v>0.6229166666666667</v>
       </c>
       <c r="K68" t="n">
-        <v>0.6444444444444446</v>
+        <v>0.6444444444444449</v>
       </c>
       <c r="L68" t="n">
         <v>2.066666666666667</v>
@@ -11002,7 +11002,7 @@
         <v>-0.8620689655172403</v>
       </c>
       <c r="AC69" t="n">
-        <v>-0.8612064737616483</v>
+        <v>-0.8612064737616476</v>
       </c>
       <c r="AD69"/>
       <c r="AE69" t="n">
@@ -11077,7 +11077,7 @@
         <v>0.6088888888888889</v>
       </c>
       <c r="K70" t="n">
-        <v>0.6533878071413061</v>
+        <v>0.6533878071413058</v>
       </c>
       <c r="L70" t="n">
         <v>1.1666666666666667</v>
@@ -11131,7 +11131,7 @@
         <v>-0.2908777969018933</v>
       </c>
       <c r="AC70" t="n">
-        <v>-0.6767764298093584</v>
+        <v>-0.6767764298093587</v>
       </c>
       <c r="AD70" t="n">
         <v>2.0</v>
@@ -11206,7 +11206,7 @@
         <v>0.5372841444270016</v>
       </c>
       <c r="K71" t="n">
-        <v>0.6716815734420243</v>
+        <v>0.6716815734420242</v>
       </c>
       <c r="L71" t="n">
         <v>2.0869565217391304</v>
@@ -11260,7 +11260,7 @@
         <v>-0.3641975308641971</v>
       </c>
       <c r="AC71" t="n">
-        <v>-0.7865353037766831</v>
+        <v>-0.7865353037766839</v>
       </c>
       <c r="AD71" t="n">
         <v>6.0</v>
@@ -11335,7 +11335,7 @@
         <v>0.42480634229000236</v>
       </c>
       <c r="K72" t="n">
-        <v>0.6736031738775605</v>
+        <v>0.6736031738775603</v>
       </c>
       <c r="L72" t="n">
         <v>3.1956521739130435</v>
@@ -11389,7 +11389,7 @@
         <v>0.14066496163682887</v>
       </c>
       <c r="AC72" t="n">
-        <v>-0.796557120500782</v>
+        <v>-0.7965571205007815</v>
       </c>
       <c r="AD72"/>
       <c r="AE72" t="n">
@@ -11464,7 +11464,7 @@
         <v>0.6607495069033531</v>
       </c>
       <c r="K73" t="n">
-        <v>0.6834720486951734</v>
+        <v>0.6834720486951736</v>
       </c>
       <c r="L73" t="n">
         <v>1.6956521739130435</v>
@@ -11518,7 +11518,7 @@
         <v>-0.40334128878281694</v>
       </c>
       <c r="AC73" t="n">
-        <v>-0.5033557046979867</v>
+        <v>-0.5033557046979854</v>
       </c>
       <c r="AD73"/>
       <c r="AE73" t="n">
@@ -11593,7 +11593,7 @@
         <v>0.5453968253968254</v>
       </c>
       <c r="K74" t="n">
-        <v>0.7200562487191552</v>
+        <v>0.7200562487191554</v>
       </c>
       <c r="L74" t="n">
         <v>3.5254237288135593</v>
@@ -11647,7 +11647,7 @@
         <v>0.6661608497723823</v>
       </c>
       <c r="AC74" t="n">
-        <v>-0.6403508771929826</v>
+        <v>-0.6403508771929823</v>
       </c>
       <c r="AD74" t="n">
         <v>2.0</v>
@@ -11722,7 +11722,7 @@
         <v>0.5151515151515151</v>
       </c>
       <c r="K75" t="n">
-        <v>0.7204348544233163</v>
+        <v>0.7204348544233167</v>
       </c>
       <c r="L75" t="n">
         <v>3.217391304347826</v>
@@ -11776,7 +11776,7 @@
         <v>-0.17391304347826014</v>
       </c>
       <c r="AC75" t="n">
-        <v>-0.5652173913043478</v>
+        <v>-0.5652173913043482</v>
       </c>
       <c r="AD75" t="n">
         <v>2.0</v>
@@ -11851,7 +11851,7 @@
         <v>0.5578703703703702</v>
       </c>
       <c r="K76" t="n">
-        <v>0.5376470418813519</v>
+        <v>0.5376470418813522</v>
       </c>
       <c r="L76" t="n">
         <v>3.5319148936170213</v>
@@ -11980,7 +11980,7 @@
         <v>0.5950413223140496</v>
       </c>
       <c r="K77" t="n">
-        <v>0.7636558774525605</v>
+        <v>0.7636558774525606</v>
       </c>
       <c r="L77" t="n">
         <v>3.5384615384615383</v>
@@ -12109,7 +12109,7 @@
         <v>0.6030245746691871</v>
       </c>
       <c r="K78" t="n">
-        <v>0.725549621864008</v>
+        <v>0.7255496218640091</v>
       </c>
       <c r="L78" t="n">
         <v>2.365079365079365</v>
@@ -12163,7 +12163,7 @@
         <v>0.46518105849582175</v>
       </c>
       <c r="AC78" t="n">
-        <v>-0.6501933820369574</v>
+        <v>-0.6501933820369566</v>
       </c>
       <c r="AD78"/>
       <c r="AE78" t="n">
@@ -12238,7 +12238,7 @@
         <v>0.5743944636678201</v>
       </c>
       <c r="K79" t="n">
-        <v>0.6684707170940085</v>
+        <v>0.6684707170940077</v>
       </c>
       <c r="L79" t="n">
         <v>1.7142857142857142</v>
@@ -12292,7 +12292,7 @@
         <v>0.44804088586030644</v>
       </c>
       <c r="AC79" t="n">
-        <v>-0.557478368355995</v>
+        <v>-0.5574783683559964</v>
       </c>
       <c r="AD79"/>
       <c r="AE79" t="n">
@@ -12367,7 +12367,7 @@
         <v>0.540495867768595</v>
       </c>
       <c r="K80" t="n">
-        <v>0.7194489972394086</v>
+        <v>0.7194489972394089</v>
       </c>
       <c r="L80" t="n">
         <v>1.4210526315789473</v>
@@ -12421,7 +12421,7 @@
         <v>-0.33333333333333304</v>
       </c>
       <c r="AC80" t="n">
-        <v>-0.19083969465648892</v>
+        <v>-0.19083969465648692</v>
       </c>
       <c r="AD80"/>
       <c r="AE80" t="n">
@@ -12496,7 +12496,7 @@
         <v>0.6136528685548294</v>
       </c>
       <c r="K81" t="n">
-        <v>0.6638037066181904</v>
+        <v>0.6638037066181907</v>
       </c>
       <c r="L81" t="n">
         <v>1.4</v>
@@ -12550,7 +12550,7 @@
         <v>0.5957446808510642</v>
       </c>
       <c r="AC81" t="n">
-        <v>-0.19206145966709323</v>
+        <v>-0.19206145966709304</v>
       </c>
       <c r="AD81" t="n">
         <v>2.0</v>
@@ -12679,7 +12679,7 @@
         <v>0.5317725752508382</v>
       </c>
       <c r="AC82" t="n">
-        <v>-0.9929119905493207</v>
+        <v>-0.9929119905493199</v>
       </c>
       <c r="AD82"/>
       <c r="AE82" t="n">
@@ -12883,7 +12883,7 @@
         <v>0.6203155818540433</v>
       </c>
       <c r="K84" t="n">
-        <v>0.6720556872697133</v>
+        <v>0.6720556872697131</v>
       </c>
       <c r="L84" t="n">
         <v>3.4918032786885247</v>
@@ -13066,7 +13066,7 @@
         <v>0.4473684210526322</v>
       </c>
       <c r="AC85" t="n">
-        <v>-0.9876543209876544</v>
+        <v>-0.9876543209876549</v>
       </c>
       <c r="AD85" t="n">
         <v>2.0</v>
@@ -13195,7 +13195,7 @@
         <v>-0.6000000000000001</v>
       </c>
       <c r="AC86" t="n">
-        <v>-0.9882491186839014</v>
+        <v>-0.9882491186839015</v>
       </c>
       <c r="AD86" t="n">
         <v>2.0</v>
@@ -13270,7 +13270,7 @@
         <v>0.2672583826429979</v>
       </c>
       <c r="K87" t="n">
-        <v>0.46503133108275946</v>
+        <v>0.4650313310827596</v>
       </c>
       <c r="L87" t="n">
         <v>5.319587628865979</v>
@@ -13399,7 +13399,7 @@
         <v>0.568870523415978</v>
       </c>
       <c r="K88" t="n">
-        <v>0.7077168106308569</v>
+        <v>0.7077168106308568</v>
       </c>
       <c r="L88" t="n">
         <v>2.5657894736842106</v>
@@ -13453,7 +13453,7 @@
         <v>0.04457142857142894</v>
       </c>
       <c r="AC88" t="n">
-        <v>-0.5397784491440079</v>
+        <v>-0.5397784491440081</v>
       </c>
       <c r="AD88"/>
       <c r="AE88" t="n">
@@ -13528,7 +13528,7 @@
         <v>0.5177335640138409</v>
       </c>
       <c r="K89" t="n">
-        <v>0.7073807095794546</v>
+        <v>0.7073807095794544</v>
       </c>
       <c r="L89" t="n">
         <v>3.3846153846153846</v>
@@ -13582,7 +13582,7 @@
         <v>0.3333333333333338</v>
       </c>
       <c r="AC89" t="n">
-        <v>-0.42292490118577064</v>
+        <v>-0.42292490118576975</v>
       </c>
       <c r="AD89"/>
       <c r="AE89" t="n">
@@ -13657,7 +13657,7 @@
         <v>0.5365079365079365</v>
       </c>
       <c r="K90" t="n">
-        <v>0.6290211899793112</v>
+        <v>0.6290211899793111</v>
       </c>
       <c r="L90" t="n">
         <v>3.5789473684210527</v>
@@ -13711,7 +13711,7 @@
         <v>0.1508379888268162</v>
       </c>
       <c r="AC90" t="n">
-        <v>-0.6825396825396824</v>
+        <v>-0.6825396825396827</v>
       </c>
       <c r="AD90" t="n">
         <v>3.0</v>
@@ -13840,7 +13840,7 @@
         <v>-0.8546042003231016</v>
       </c>
       <c r="AC91" t="n">
-        <v>-0.9444444444444444</v>
+        <v>-0.9444444444444448</v>
       </c>
       <c r="AD91"/>
       <c r="AE91" t="n">
@@ -13915,7 +13915,7 @@
         <v>0.2923585950080515</v>
       </c>
       <c r="K92" t="n">
-        <v>0.7366006846712263</v>
+        <v>0.7366006846712262</v>
       </c>
       <c r="L92" t="n">
         <v>5.32319391634981</v>
@@ -13969,7 +13969,7 @@
         <v>0.2770618556701038</v>
       </c>
       <c r="AC92" t="n">
-        <v>-0.31656548135299245</v>
+        <v>-0.31656548135299345</v>
       </c>
       <c r="AD92" t="n">
         <v>2.0</v>
@@ -14044,7 +14044,7 @@
         <v>0.5997395833333333</v>
       </c>
       <c r="K93" t="n">
-        <v>0.6964745865440548</v>
+        <v>0.6964745865440547</v>
       </c>
       <c r="L93" t="n">
         <v>1.90625</v>
@@ -14098,7 +14098,7 @@
         <v>-0.7169650468883203</v>
       </c>
       <c r="AC93" t="n">
-        <v>-0.7280825128926396</v>
+        <v>-0.7280825128926394</v>
       </c>
       <c r="AD93" t="n">
         <v>8.0</v>
@@ -14173,7 +14173,7 @@
         <v>0.6217687074829932</v>
       </c>
       <c r="K94" t="n">
-        <v>0.8011677544593898</v>
+        <v>0.8011677544593905</v>
       </c>
       <c r="L94" t="n">
         <v>3.086206896551724</v>
@@ -14227,7 +14227,7 @@
         <v>0.28829686013320743</v>
       </c>
       <c r="AC94" t="n">
-        <v>-0.6146265560165977</v>
+        <v>-0.6146265560165979</v>
       </c>
       <c r="AD94" t="n">
         <v>2.0</v>
@@ -14356,7 +14356,7 @@
         <v>0.499999999999996</v>
       </c>
       <c r="AC95" t="n">
-        <v>-0.694267515923567</v>
+        <v>-0.6942675159235668</v>
       </c>
       <c r="AD95"/>
       <c r="AE95" t="n">
@@ -14431,7 +14431,7 @@
         <v>0.5047619047619047</v>
       </c>
       <c r="K96" t="n">
-        <v>0.6568028603790268</v>
+        <v>0.6568028603790264</v>
       </c>
       <c r="L96" t="n">
         <v>1.836734693877551</v>
@@ -14485,7 +14485,7 @@
         <v>0.10937500000000033</v>
       </c>
       <c r="AC96" t="n">
-        <v>-0.7910278250993755</v>
+        <v>-0.7910278250993759</v>
       </c>
       <c r="AD96"/>
       <c r="AE96" t="n">
@@ -14560,7 +14560,7 @@
         <v>0.5575520833333333</v>
       </c>
       <c r="K97" t="n">
-        <v>0.7219433793087969</v>
+        <v>0.7219433793087967</v>
       </c>
       <c r="L97" t="n">
         <v>2.0</v>
@@ -14689,7 +14689,7 @@
         <v>0.5039246467817896</v>
       </c>
       <c r="K98" t="n">
-        <v>0.7716570891889998</v>
+        <v>0.7716570891890003</v>
       </c>
       <c r="L98" t="n">
         <v>3.727272727272727</v>
@@ -14872,7 +14872,7 @@
         <v>-0.12785388127853828</v>
       </c>
       <c r="AC99" t="n">
-        <v>-0.5890083632019112</v>
+        <v>-0.5890083632019113</v>
       </c>
       <c r="AD99" t="n">
         <v>2.0</v>
@@ -14947,7 +14947,7 @@
         <v>0.4679930795847751</v>
       </c>
       <c r="K100" t="n">
-        <v>0.634190019720194</v>
+        <v>0.6341900197201942</v>
       </c>
       <c r="L100" t="n">
         <v>1.631578947368421</v>
@@ -15001,7 +15001,7 @@
         <v>0.09174311926605427</v>
       </c>
       <c r="AC100" t="n">
-        <v>-0.6116279069767444</v>
+        <v>-0.6116279069767443</v>
       </c>
       <c r="AD100"/>
       <c r="AE100" t="n">
@@ -15130,7 +15130,7 @@
         <v>-0.3619047619047624</v>
       </c>
       <c r="AC101" t="n">
-        <v>-0.6970711297071127</v>
+        <v>-0.6970711297071128</v>
       </c>
       <c r="AD101" t="n">
         <v>2.0</v>
@@ -15205,7 +15205,7 @@
         <v>0.32007575757575757</v>
       </c>
       <c r="K102" t="n">
-        <v>0.5575331000518126</v>
+        <v>0.5575331000518123</v>
       </c>
       <c r="L102" t="n">
         <v>2.3157894736842106</v>
@@ -15259,7 +15259,7 @@
         <v>0.13043478260869532</v>
       </c>
       <c r="AC102" t="n">
-        <v>-0.38307552320291083</v>
+        <v>-0.383075523202912</v>
       </c>
       <c r="AD102" t="n">
         <v>6.0</v>
@@ -15334,7 +15334,7 @@
         <v>0.6203155818540433</v>
       </c>
       <c r="K103" t="n">
-        <v>0.7838946728446441</v>
+        <v>0.7838946728446438</v>
       </c>
       <c r="L103" t="n">
         <v>2.5161290322580645</v>
@@ -15388,7 +15388,7 @@
         <v>-0.5589941972920696</v>
       </c>
       <c r="AC103" t="n">
-        <v>-0.7644710578842315</v>
+        <v>-0.7644710578842316</v>
       </c>
       <c r="AD103" t="n">
         <v>2.0</v>
@@ -15463,7 +15463,7 @@
         <v>0.11589402355792013</v>
       </c>
       <c r="K104" t="n">
-        <v>0.43249991370841584</v>
+        <v>0.4324999137084158</v>
       </c>
       <c r="L104" t="n">
         <v>4.375722543352601</v>
@@ -15517,7 +15517,7 @@
         <v>0.2698591549295773</v>
       </c>
       <c r="AC104" t="n">
-        <v>0.08920021280368971</v>
+        <v>0.08920021280368959</v>
       </c>
       <c r="AD104" t="n">
         <v>7.0</v>
@@ -15646,7 +15646,7 @@
         <v>-0.07547169811321</v>
       </c>
       <c r="AC105" t="n">
-        <v>-0.12000000000000002</v>
+        <v>-0.11999999999999936</v>
       </c>
       <c r="AD105"/>
       <c r="AE105" t="n">
@@ -15719,7 +15719,7 @@
         <v>0.500865051903114</v>
       </c>
       <c r="K106" t="n">
-        <v>0.6543696995514867</v>
+        <v>0.6543696995514879</v>
       </c>
       <c r="L106" t="n">
         <v>2.546875</v>
@@ -15773,7 +15773,7 @@
         <v>-0.0384615384615372</v>
       </c>
       <c r="AC106" t="n">
-        <v>-0.6074672048435917</v>
+        <v>-0.6074672048435906</v>
       </c>
       <c r="AD106"/>
       <c r="AE106" t="n">
@@ -15902,7 +15902,7 @@
         <v>-0.15384615384615388</v>
       </c>
       <c r="AC107" t="n">
-        <v>-0.3964285714285716</v>
+        <v>-0.39642857142857185</v>
       </c>
       <c r="AD107" t="n">
         <v>2.0</v>
@@ -15977,7 +15977,7 @@
         <v>0.46044936903662664</v>
       </c>
       <c r="K108" t="n">
-        <v>0.703183065392293</v>
+        <v>0.7031830653922929</v>
       </c>
       <c r="L108" t="n">
         <v>4.101351351351352</v>
@@ -16031,7 +16031,7 @@
         <v>-0.32330827067669143</v>
       </c>
       <c r="AC108" t="n">
-        <v>-0.11022272986864685</v>
+        <v>-0.11022272986864656</v>
       </c>
       <c r="AD108"/>
       <c r="AE108" t="n">
@@ -16106,7 +16106,7 @@
         <v>0.706828885400314</v>
       </c>
       <c r="K109" t="n">
-        <v>0.7465589852152265</v>
+        <v>0.7465589852152268</v>
       </c>
       <c r="L109" t="n">
         <v>1.625</v>
@@ -16160,7 +16160,7 @@
         <v>-0.5094339622641518</v>
       </c>
       <c r="AC109" t="n">
-        <v>-0.9073518379594899</v>
+        <v>-0.9073518379594895</v>
       </c>
       <c r="AD109" t="n">
         <v>2.0</v>
@@ -16235,7 +16235,7 @@
         <v>0.6554160125588697</v>
       </c>
       <c r="K110" t="n">
-        <v>0.7781497533091724</v>
+        <v>0.7781497533091725</v>
       </c>
       <c r="L110" t="n">
         <v>3.1346153846153846</v>
@@ -16289,7 +16289,7 @@
         <v>-0.415228426395938</v>
       </c>
       <c r="AC110" t="n">
-        <v>-0.7953795379537955</v>
+        <v>-0.7953795379537946</v>
       </c>
       <c r="AD110" t="n">
         <v>2.0</v>
@@ -16364,7 +16364,7 @@
         <v>0.41738754325259514</v>
       </c>
       <c r="K111" t="n">
-        <v>0.5932868346495678</v>
+        <v>0.5932868346495671</v>
       </c>
       <c r="L111" t="n">
         <v>2.586206896551724</v>
@@ -16493,7 +16493,7 @@
         <v>0.6214876033057851</v>
       </c>
       <c r="K112" t="n">
-        <v>0.6848446400614068</v>
+        <v>0.6848446400614071</v>
       </c>
       <c r="L112" t="n">
         <v>1.5217391304347827</v>
@@ -16547,7 +16547,7 @@
         <v>-0.22222222222222177</v>
       </c>
       <c r="AC112" t="n">
-        <v>-0.9616666666666671</v>
+        <v>-0.9616666666666669</v>
       </c>
       <c r="AD112"/>
       <c r="AE112" t="n">
@@ -16676,7 +16676,7 @@
         <v>0.054892601431978084</v>
       </c>
       <c r="AC113" t="n">
-        <v>-0.28398384925975756</v>
+        <v>-0.28398384925975745</v>
       </c>
       <c r="AD113"/>
       <c r="AE113" t="n">
@@ -16805,7 +16805,7 @@
         <v>-0.621505376344086</v>
       </c>
       <c r="AC114" t="n">
-        <v>-0.9753381066030233</v>
+        <v>-0.9753381066030232</v>
       </c>
       <c r="AD114"/>
       <c r="AE114" t="n">
@@ -16880,7 +16880,7 @@
         <v>0.6067503924646782</v>
       </c>
       <c r="K115" t="n">
-        <v>0.7605622429272167</v>
+        <v>0.7605622429272175</v>
       </c>
       <c r="L115" t="n">
         <v>1.9565217391304348</v>
@@ -16934,7 +16934,7 @@
         <v>0.600000000000001</v>
       </c>
       <c r="AC115" t="n">
-        <v>-0.7662337662337664</v>
+        <v>-0.7662337662337659</v>
       </c>
       <c r="AD115"/>
       <c r="AE115" t="n">
@@ -17009,7 +17009,7 @@
         <v>0.7095761381475667</v>
       </c>
       <c r="K116" t="n">
-        <v>0.640603345442122</v>
+        <v>0.6406033454421217</v>
       </c>
       <c r="L116" t="n">
         <v>2.4693877551020407</v>
@@ -17138,7 +17138,7 @@
         <v>0.47107438016528924</v>
       </c>
       <c r="K117" t="n">
-        <v>0.5522465746544815</v>
+        <v>0.5522465746544817</v>
       </c>
       <c r="L117" t="n">
         <v>1.5</v>
@@ -17267,7 +17267,7 @@
         <v>0.4832347140039448</v>
       </c>
       <c r="K118" t="n">
-        <v>0.7323990412506669</v>
+        <v>0.7323990412506672</v>
       </c>
       <c r="L118" t="n">
         <v>2.4464285714285716</v>
@@ -17396,7 +17396,7 @@
         <v>0.6883830455259027</v>
       </c>
       <c r="K119" t="n">
-        <v>0.7670059672747956</v>
+        <v>0.7670059672747953</v>
       </c>
       <c r="L119" t="n">
         <v>2.289473684210526</v>
@@ -17450,7 +17450,7 @@
         <v>0.505300353356888</v>
       </c>
       <c r="AC119" t="n">
-        <v>-0.9444444444444444</v>
+        <v>-0.9444444444444448</v>
       </c>
       <c r="AD119" t="n">
         <v>2.0</v>
@@ -17525,7 +17525,7 @@
         <v>0.6607495069033531</v>
       </c>
       <c r="K120" t="n">
-        <v>0.7107858251581546</v>
+        <v>0.7107858251581548</v>
       </c>
       <c r="L120" t="n">
         <v>2.1739130434782608</v>
@@ -17579,7 +17579,7 @@
         <v>-0.4666666666666668</v>
       </c>
       <c r="AC120" t="n">
-        <v>-0.9398998330550921</v>
+        <v>-0.9398998330550923</v>
       </c>
       <c r="AD120"/>
       <c r="AE120" t="n">
@@ -17654,7 +17654,7 @@
         <v>0.5986159169550173</v>
       </c>
       <c r="K121" t="n">
-        <v>0.6677393407133915</v>
+        <v>0.6677393407133918</v>
       </c>
       <c r="L121" t="n">
         <v>2.617021276595745</v>
@@ -17708,7 +17708,7 @@
         <v>0.8997493734335827</v>
       </c>
       <c r="AC121" t="n">
-        <v>-0.49659863945578236</v>
+        <v>-0.4965986394557827</v>
       </c>
       <c r="AD121" t="n">
         <v>2.0</v>
@@ -17783,7 +17783,7 @@
         <v>0.6125360964837778</v>
       </c>
       <c r="K122" t="n">
-        <v>0.8149605674668184</v>
+        <v>0.8149605674668174</v>
       </c>
       <c r="L122" t="n">
         <v>2.1192660550458715</v>
@@ -17837,7 +17837,7 @@
         <v>0.1717461455718907</v>
       </c>
       <c r="AC122" t="n">
-        <v>-0.30882089819287895</v>
+        <v>-0.3088208981928793</v>
       </c>
       <c r="AD122" t="n">
         <v>2.0</v>
@@ -17912,7 +17912,7 @@
         <v>0.5255208333333333</v>
       </c>
       <c r="K123" t="n">
-        <v>0.6775443814180122</v>
+        <v>0.6775443814180118</v>
       </c>
       <c r="L123" t="n">
         <v>2.051282051282051</v>
@@ -17966,7 +17966,7 @@
         <v>0.3469910371318811</v>
       </c>
       <c r="AC123" t="n">
-        <v>-0.25445292620865134</v>
+        <v>-0.2544529262086522</v>
       </c>
       <c r="AD123" t="n">
         <v>2.0</v>
@@ -18041,7 +18041,7 @@
         <v>0.6372549019607843</v>
       </c>
       <c r="K124" t="n">
-        <v>0.6651706006880543</v>
+        <v>0.665170600688054</v>
       </c>
       <c r="L124" t="n">
         <v>1.6666666666666667</v>
@@ -18095,7 +18095,7 @@
         <v>0.6078431372549021</v>
       </c>
       <c r="AC124" t="n">
-        <v>-0.9968360688155028</v>
+        <v>-0.996836068815503</v>
       </c>
       <c r="AD124" t="n">
         <v>2.0</v>
@@ -18170,7 +18170,7 @@
         <v>0.41983471074380163</v>
       </c>
       <c r="K125" t="n">
-        <v>0.5471466884461431</v>
+        <v>0.5471466884461432</v>
       </c>
       <c r="L125" t="n">
         <v>2.6551724137931036</v>
@@ -18299,7 +18299,7 @@
         <v>0.5374753451676528</v>
       </c>
       <c r="K126" t="n">
-        <v>0.6553268404232157</v>
+        <v>0.6553268404232168</v>
       </c>
       <c r="L126" t="n">
         <v>1.7954545454545454</v>
@@ -18428,7 +18428,7 @@
         <v>0.4006076388888889</v>
       </c>
       <c r="K127" t="n">
-        <v>0.5352996816101626</v>
+        <v>0.5352996816101624</v>
       </c>
       <c r="L127" t="n">
         <v>1.9622641509433962</v>
@@ -18482,7 +18482,7 @@
         <v>-0.470631970260224</v>
       </c>
       <c r="AC127" t="n">
-        <v>-0.5966487133453016</v>
+        <v>-0.5966487133453022</v>
       </c>
       <c r="AD127"/>
       <c r="AE127" t="n">
@@ -18557,7 +18557,7 @@
         <v>0.5670445956160242</v>
       </c>
       <c r="K128" t="n">
-        <v>0.7520380747830199</v>
+        <v>0.7520380747830189</v>
       </c>
       <c r="L128" t="n">
         <v>2.8666666666666667</v>
@@ -18611,7 +18611,7 @@
         <v>0.15850702859912777</v>
       </c>
       <c r="AC128" t="n">
-        <v>-0.5568464730290459</v>
+        <v>-0.5568464730290458</v>
       </c>
       <c r="AD128"/>
       <c r="AE128" t="n">
@@ -18740,7 +18740,7 @@
         <v>0.5652173913043476</v>
       </c>
       <c r="AC129" t="n">
-        <v>-0.9103773584905662</v>
+        <v>-0.9103773584905657</v>
       </c>
       <c r="AD129" t="n">
         <v>2.0</v>
@@ -18815,7 +18815,7 @@
         <v>0.25570586820586816</v>
       </c>
       <c r="K130" t="n">
-        <v>0.3337674828751594</v>
+        <v>0.3337674828751593</v>
       </c>
       <c r="L130" t="n">
         <v>3.0357142857142856</v>
@@ -18869,7 +18869,7 @@
         <v>0.5324675324675326</v>
       </c>
       <c r="AC130" t="n">
-        <v>-0.22981366459627287</v>
+        <v>-0.22981366459627858</v>
       </c>
       <c r="AD130" t="n">
         <v>3.0</v>
@@ -18998,7 +18998,7 @@
         <v>0.26923076923076966</v>
       </c>
       <c r="AC131" t="n">
-        <v>-0.5759917568263787</v>
+        <v>-0.5759917568263775</v>
       </c>
       <c r="AD131" t="n">
         <v>3.0</v>
@@ -19073,7 +19073,7 @@
         <v>0.5166666666666667</v>
       </c>
       <c r="K132" t="n">
-        <v>0.6361776167253989</v>
+        <v>0.6361776167253992</v>
       </c>
       <c r="L132" t="n">
         <v>1.4</v>
@@ -19127,7 +19127,7 @@
         <v>-0.4579439252336446</v>
       </c>
       <c r="AC132" t="n">
-        <v>-0.5416666666666667</v>
+        <v>-0.5416666666666665</v>
       </c>
       <c r="AD132" t="n">
         <v>3.0</v>
@@ -19202,7 +19202,7 @@
         <v>0.5096153846153846</v>
       </c>
       <c r="K133" t="n">
-        <v>0.6908948344366225</v>
+        <v>0.6908948344366226</v>
       </c>
       <c r="L133" t="n">
         <v>1.625</v>
@@ -19256,7 +19256,7 @@
         <v>0.5952380952380918</v>
       </c>
       <c r="AC133" t="n">
-        <v>-0.5454545454545453</v>
+        <v>-0.545454545454545</v>
       </c>
       <c r="AD133" t="n">
         <v>4.0</v>
@@ -19331,7 +19331,7 @@
         <v>0.4359375</v>
       </c>
       <c r="K134" t="n">
-        <v>0.6796519675925619</v>
+        <v>0.6796519675925623</v>
       </c>
       <c r="L134" t="n">
         <v>1.7435897435897436</v>
@@ -19385,7 +19385,7 @@
         <v>0.5887850467289721</v>
       </c>
       <c r="AC134" t="n">
-        <v>-0.14893617021276598</v>
+        <v>-0.14893617021276556</v>
       </c>
       <c r="AD134" t="n">
         <v>4.0</v>
@@ -19460,7 +19460,7 @@
         <v>0.7508650519031141</v>
       </c>
       <c r="K135" t="n">
-        <v>0.7559749739472219</v>
+        <v>0.7559749739472221</v>
       </c>
       <c r="L135" t="n">
         <v>3.4107142857142856</v>
@@ -19514,7 +19514,7 @@
         <v>0.387755102040817</v>
       </c>
       <c r="AC135" t="n">
-        <v>-0.4480089876419924</v>
+        <v>-0.4480089876419919</v>
       </c>
       <c r="AD135" t="n">
         <v>5.0</v>
@@ -19589,7 +19589,7 @@
         <v>0.616370808678501</v>
       </c>
       <c r="K136" t="n">
-        <v>0.7280452596986553</v>
+        <v>0.7280452596986559</v>
       </c>
       <c r="L136" t="n">
         <v>1.5454545454545454</v>
@@ -19643,7 +19643,7 @@
         <v>0.8656126482213412</v>
       </c>
       <c r="AC136" t="n">
-        <v>-0.6451612903225803</v>
+        <v>-0.6451612903225804</v>
       </c>
       <c r="AD136" t="n">
         <v>2.0</v>
@@ -19718,7 +19718,7 @@
         <v>0.5925925925925926</v>
       </c>
       <c r="K137" t="n">
-        <v>0.5242080512939442</v>
+        <v>0.5242080512939441</v>
       </c>
       <c r="L137" t="n">
         <v>2.4074074074074074</v>
@@ -19847,7 +19847,7 @@
         <v>0.5545729402872259</v>
       </c>
       <c r="K138" t="n">
-        <v>0.7850146706758379</v>
+        <v>0.785014670675838</v>
       </c>
       <c r="L138" t="n">
         <v>3.338235294117647</v>
@@ -19901,7 +19901,7 @@
         <v>-0.0067924528301877615</v>
       </c>
       <c r="AC138" t="n">
-        <v>-0.2790697674418605</v>
+        <v>-0.27906976744186046</v>
       </c>
       <c r="AD138"/>
       <c r="AE138" t="n">
@@ -19976,7 +19976,7 @@
         <v>0.6009440813362382</v>
       </c>
       <c r="K139" t="n">
-        <v>0.6389302142172326</v>
+        <v>0.6389302142172324</v>
       </c>
       <c r="L139" t="n">
         <v>2.9714285714285715</v>
@@ -20030,7 +20030,7 @@
         <v>-0.009345794392523633</v>
       </c>
       <c r="AC139" t="n">
-        <v>-0.5157894736842104</v>
+        <v>-0.515789473684211</v>
       </c>
       <c r="AD139" t="n">
         <v>3.0</v>
@@ -20105,7 +20105,7 @@
         <v>0.4217171717171717</v>
       </c>
       <c r="K140" t="n">
-        <v>0.603124493497912</v>
+        <v>0.6031244934979114</v>
       </c>
       <c r="L140" t="n">
         <v>2.1714285714285713</v>
@@ -20159,7 +20159,7 @@
         <v>-0.1111111111111111</v>
       </c>
       <c r="AC140" t="n">
-        <v>0.16666666666666574</v>
+        <v>0.16666666666666505</v>
       </c>
       <c r="AD140"/>
       <c r="AE140" t="n">
@@ -20234,7 +20234,7 @@
         <v>0.6216412490922295</v>
       </c>
       <c r="K141" t="n">
-        <v>0.6548896519663272</v>
+        <v>0.6548896519663271</v>
       </c>
       <c r="L141" t="n">
         <v>5.052083333333333</v>
@@ -20288,7 +20288,7 @@
         <v>0.4149512459371604</v>
       </c>
       <c r="AC141" t="n">
-        <v>-0.6549586776859505</v>
+        <v>-0.6549586776859507</v>
       </c>
       <c r="AD141" t="n">
         <v>4.0</v>
@@ -20363,7 +20363,7 @@
         <v>0.620242214532872</v>
       </c>
       <c r="K142" t="n">
-        <v>0.6839268025096327</v>
+        <v>0.6839268025096328</v>
       </c>
       <c r="L142" t="n">
         <v>1.4482758620689655</v>
@@ -20417,7 +20417,7 @@
         <v>0.325383304940375</v>
       </c>
       <c r="AC142" t="n">
-        <v>-0.6639308855291578</v>
+        <v>-0.6639308855291577</v>
       </c>
       <c r="AD142"/>
       <c r="AE142" t="n">
@@ -20621,7 +20621,7 @@
         <v>0.5644444444444444</v>
       </c>
       <c r="K144" t="n">
-        <v>0.743576418960531</v>
+        <v>0.7435764189605306</v>
       </c>
       <c r="L144" t="n">
         <v>2.217391304347826</v>
@@ -20675,7 +20675,7 @@
         <v>0.34193548387096895</v>
       </c>
       <c r="AC144" t="n">
-        <v>-0.552016985138004</v>
+        <v>-0.5520169851380039</v>
       </c>
       <c r="AD144" t="n">
         <v>3.0</v>
@@ -20750,7 +20750,7 @@
         <v>1.0</v>
       </c>
       <c r="K145" t="n">
-        <v>0.7759907622602042</v>
+        <v>0.7759907622602039</v>
       </c>
       <c r="L145" t="n">
         <v>2.71875</v>
@@ -20875,7 +20875,7 @@
         <v>0.5621708850008494</v>
       </c>
       <c r="K146" t="n">
-        <v>0.723062279606614</v>
+        <v>0.7230622796066136</v>
       </c>
       <c r="L146" t="n">
         <v>4.60655737704918</v>
@@ -21058,7 +21058,7 @@
         <v>-0.6540540540540537</v>
       </c>
       <c r="AC147" t="n">
-        <v>-0.9875621890547264</v>
+        <v>-0.9875621890547257</v>
       </c>
       <c r="AD147" t="n">
         <v>2.0</v>
@@ -21133,7 +21133,7 @@
         <v>0.5051903114186851</v>
       </c>
       <c r="K148" t="n">
-        <v>0.46873894098876523</v>
+        <v>0.468738940988765</v>
       </c>
       <c r="L148" t="n">
         <v>3.2363636363636363</v>
@@ -21187,7 +21187,7 @@
         <v>0.7600000000000005</v>
       </c>
       <c r="AC148" t="n">
-        <v>-0.8902147971360386</v>
+        <v>-0.8902147971360387</v>
       </c>
       <c r="AD148" t="n">
         <v>3.0</v>
@@ -21262,7 +21262,7 @@
         <v>0.4677685950413223</v>
       </c>
       <c r="K149" t="n">
-        <v>0.6363346460488312</v>
+        <v>0.636334646048831</v>
       </c>
       <c r="L149" t="n">
         <v>1.7058823529411764</v>
@@ -21316,7 +21316,7 @@
         <v>0.3399999999999991</v>
       </c>
       <c r="AC149" t="n">
-        <v>-0.8507936507936505</v>
+        <v>-0.8507936507936514</v>
       </c>
       <c r="AD149"/>
       <c r="AE149" t="n">
@@ -21391,7 +21391,7 @@
         <v>0.6254325259515571</v>
       </c>
       <c r="K150" t="n">
-        <v>0.8167107515573924</v>
+        <v>0.8167107515573926</v>
       </c>
       <c r="L150" t="n">
         <v>2.119047619047619</v>
@@ -21445,7 +21445,7 @@
         <v>-0.5394566623544641</v>
       </c>
       <c r="AC150" t="n">
-        <v>-0.6183274021352313</v>
+        <v>-0.6183274021352311</v>
       </c>
       <c r="AD150" t="n">
         <v>2.0</v>
@@ -21520,7 +21520,7 @@
         <v>0.6088888888888889</v>
       </c>
       <c r="K151" t="n">
-        <v>0.653387807141306</v>
+        <v>0.6533878071413058</v>
       </c>
       <c r="L151" t="n">
         <v>3.090909090909091</v>
@@ -21574,7 +21574,7 @@
         <v>-0.25000000000000017</v>
       </c>
       <c r="AC151" t="n">
-        <v>-0.6767764298093584</v>
+        <v>-0.6767764298093587</v>
       </c>
       <c r="AD151" t="n">
         <v>2.0</v>
@@ -21703,7 +21703,7 @@
         <v>-0.3161290322580655</v>
       </c>
       <c r="AC152" t="n">
-        <v>-0.9814814814814814</v>
+        <v>-0.9814814814814817</v>
       </c>
       <c r="AD152" t="n">
         <v>2.0</v>
@@ -21778,7 +21778,7 @@
         <v>0.8177777777777778</v>
       </c>
       <c r="K153" t="n">
-        <v>0.6766248927741227</v>
+        <v>0.6766248927741222</v>
       </c>
       <c r="L153" t="n">
         <v>1.8085106382978724</v>
@@ -21903,7 +21903,7 @@
         <v>0.6351084812623274</v>
       </c>
       <c r="K154" t="n">
-        <v>0.6921410326398417</v>
+        <v>0.6921410326398418</v>
       </c>
       <c r="L154" t="n">
         <v>3.7857142857142856</v>
@@ -21955,7 +21955,7 @@
       </c>
       <c r="AB154"/>
       <c r="AC154" t="n">
-        <v>-0.5542938254080909</v>
+        <v>-0.5542938254080911</v>
       </c>
       <c r="AD154"/>
       <c r="AE154" t="n">
@@ -22159,7 +22159,7 @@
         <v>0.5453648915187377</v>
       </c>
       <c r="K156" t="n">
-        <v>0.5729944499546029</v>
+        <v>0.5729944499546028</v>
       </c>
       <c r="L156" t="n">
         <v>2.28125</v>
@@ -22213,7 +22213,7 @@
         <v>0.17803660565724017</v>
       </c>
       <c r="AC156" t="n">
-        <v>-0.7175141242937855</v>
+        <v>-0.7175141242937852</v>
       </c>
       <c r="AD156"/>
       <c r="AE156" t="n">
@@ -22288,7 +22288,7 @@
         <v>0.5820707070707071</v>
       </c>
       <c r="K157" t="n">
-        <v>0.6749707165392153</v>
+        <v>0.6749707165392146</v>
       </c>
       <c r="L157" t="n">
         <v>2.269230769230769</v>
@@ -22342,7 +22342,7 @@
         <v>-0.42857142857142844</v>
       </c>
       <c r="AC157" t="n">
-        <v>-0.8502994011976052</v>
+        <v>-0.8502994011976053</v>
       </c>
       <c r="AD157" t="n">
         <v>3.0</v>
@@ -22417,7 +22417,7 @@
         <v>0.5877712031558185</v>
       </c>
       <c r="K158" t="n">
-        <v>0.655205145344012</v>
+        <v>0.6552051453440119</v>
       </c>
       <c r="L158" t="n">
         <v>3.8541666666666665</v>
@@ -22471,7 +22471,7 @@
         <v>0.13627639155470234</v>
       </c>
       <c r="AC158" t="n">
-        <v>-0.9760479041916169</v>
+        <v>-0.9760479041916166</v>
       </c>
       <c r="AD158" t="n">
         <v>2.0</v>
@@ -22600,7 +22600,7 @@
         <v>0.013054830287205348</v>
       </c>
       <c r="AC159" t="n">
-        <v>-0.5526066350710903</v>
+        <v>-0.5526066350710911</v>
       </c>
       <c r="AD159"/>
       <c r="AE159" t="n">
@@ -22675,7 +22675,7 @@
         <v>0.6043956043956044</v>
       </c>
       <c r="K160" t="n">
-        <v>0.6192501947457052</v>
+        <v>0.6192501947457054</v>
       </c>
       <c r="L160" t="n">
         <v>1.4615384615384615</v>
@@ -22729,7 +22729,7 @@
         <v>-0.7411764705882351</v>
       </c>
       <c r="AC160" t="n">
-        <v>-0.9929119905493207</v>
+        <v>-0.9929119905493199</v>
       </c>
       <c r="AD160" t="n">
         <v>2.0</v>
@@ -22804,7 +22804,7 @@
         <v>0.591715976331361</v>
       </c>
       <c r="K161" t="n">
-        <v>0.7009578627995708</v>
+        <v>0.7009578627995711</v>
       </c>
       <c r="L161" t="n">
         <v>2.4166666666666665</v>
@@ -22987,7 +22987,7 @@
         <v>0.623471882640587</v>
       </c>
       <c r="AC162" t="n">
-        <v>-0.6991869918699187</v>
+        <v>-0.6991869918699213</v>
       </c>
       <c r="AD162"/>
       <c r="AE162" t="n">
@@ -23191,7 +23191,7 @@
         <v>0.28479709473694903</v>
       </c>
       <c r="K164" t="n">
-        <v>0.6055530991185532</v>
+        <v>0.6055530991185533</v>
       </c>
       <c r="L164" t="n">
         <v>4.278884462151394</v>
@@ -23245,7 +23245,7 @@
         <v>-0.6775262286029815</v>
       </c>
       <c r="AC164" t="n">
-        <v>-0.6759202453987734</v>
+        <v>-0.6759202453987739</v>
       </c>
       <c r="AD164"/>
       <c r="AE164" t="n">
@@ -23374,7 +23374,7 @@
         <v>-0.71007371007371</v>
       </c>
       <c r="AC165" t="n">
-        <v>-0.9224489795918367</v>
+        <v>-0.9224489795918362</v>
       </c>
       <c r="AD165"/>
       <c r="AE165" t="n">
@@ -23449,7 +23449,7 @@
         <v>0.5694444444444444</v>
       </c>
       <c r="K166" t="n">
-        <v>0.7295283117584016</v>
+        <v>0.7295283117584019</v>
       </c>
       <c r="L166" t="n">
         <v>1.8636363636363635</v>
@@ -23503,7 +23503,7 @@
         <v>0.0730643402399123</v>
       </c>
       <c r="AC166" t="n">
-        <v>-0.6746268656716422</v>
+        <v>-0.6746268656716424</v>
       </c>
       <c r="AD166"/>
       <c r="AE166" t="n">
@@ -23578,7 +23578,7 @@
         <v>0.44666666666666666</v>
       </c>
       <c r="K167" t="n">
-        <v>0.5138798723099931</v>
+        <v>0.5138798723099929</v>
       </c>
       <c r="L167" t="n">
         <v>1.72</v>
@@ -23632,7 +23632,7 @@
         <v>-0.2764505119453922</v>
       </c>
       <c r="AC167" t="n">
-        <v>-0.8906249999999996</v>
+        <v>-0.8906249999999997</v>
       </c>
       <c r="AD167" t="n">
         <v>2.0</v>
@@ -23707,7 +23707,7 @@
         <v>0.46745562130177515</v>
       </c>
       <c r="K168" t="n">
-        <v>0.5914481721951657</v>
+        <v>0.591448172195166</v>
       </c>
       <c r="L168" t="n">
         <v>3.150943396226415</v>
@@ -23761,7 +23761,7 @@
         <v>-0.6412078152753112</v>
       </c>
       <c r="AC168" t="n">
-        <v>-0.8114343029087261</v>
+        <v>-0.8114343029087258</v>
       </c>
       <c r="AD168"/>
       <c r="AE168" t="n">
@@ -23836,7 +23836,7 @@
         <v>0.4478021978021978</v>
       </c>
       <c r="K169" t="n">
-        <v>0.6651282312391135</v>
+        <v>0.6651282312391141</v>
       </c>
       <c r="L169" t="n">
         <v>2.14</v>
@@ -23890,7 +23890,7 @@
         <v>-0.06583072100313452</v>
       </c>
       <c r="AC169" t="n">
-        <v>-0.5148063781321186</v>
+        <v>-0.5148063781321187</v>
       </c>
       <c r="AD169"/>
       <c r="AE169" t="n">
@@ -23965,7 +23965,7 @@
         <v>0.40927021696252464</v>
       </c>
       <c r="K170" t="n">
-        <v>0.5555541941161155</v>
+        <v>0.5555541941161156</v>
       </c>
       <c r="L170" t="n">
         <v>2.0</v>
@@ -24019,7 +24019,7 @@
         <v>0.4680851063829787</v>
       </c>
       <c r="AC170" t="n">
-        <v>-0.3469387755102046</v>
+        <v>-0.34693877551020375</v>
       </c>
       <c r="AD170"/>
       <c r="AE170" t="n">
@@ -24148,7 +24148,7 @@
         <v>0.08212560386473433</v>
       </c>
       <c r="AC171" t="n">
-        <v>-0.42449125312388397</v>
+        <v>-0.4244912531238837</v>
       </c>
       <c r="AD171" t="n">
         <v>2.0</v>
@@ -24223,7 +24223,7 @@
         <v>0.5808080808080808</v>
       </c>
       <c r="K172" t="n">
-        <v>0.6896139328800207</v>
+        <v>0.6896139328800206</v>
       </c>
       <c r="L172" t="n">
         <v>1.0</v>
@@ -24277,7 +24277,7 @@
         <v>-0.5738498789346241</v>
       </c>
       <c r="AC172" t="n">
-        <v>-0.9066666666666664</v>
+        <v>-0.9066666666666662</v>
       </c>
       <c r="AD172" t="n">
         <v>2.0</v>
@@ -24406,7 +24406,7 @@
         <v>-0.06552706552706536</v>
       </c>
       <c r="AC173" t="n">
-        <v>-0.6244430299172499</v>
+        <v>-0.6244430299172504</v>
       </c>
       <c r="AD173"/>
       <c r="AE173" t="n">
@@ -24481,7 +24481,7 @@
         <v>0.653968253968254</v>
       </c>
       <c r="K174" t="n">
-        <v>0.7273681331479638</v>
+        <v>0.727368133147963</v>
       </c>
       <c r="L174" t="n">
         <v>3.4705882352941178</v>
@@ -24535,7 +24535,7 @@
         <v>-0.6344463971880495</v>
       </c>
       <c r="AC174" t="n">
-        <v>-0.9829424307036247</v>
+        <v>-0.9829424307036243</v>
       </c>
       <c r="AD174" t="n">
         <v>2.0</v>
@@ -24610,7 +24610,7 @@
         <v>0.6059654631083202</v>
       </c>
       <c r="K175" t="n">
-        <v>0.7023888300243784</v>
+        <v>0.702388830024379</v>
       </c>
       <c r="L175" t="n">
         <v>2.6206896551724137</v>
@@ -24739,7 +24739,7 @@
         <v>0.5277777777777778</v>
       </c>
       <c r="K176" t="n">
-        <v>0.5497246451155332</v>
+        <v>0.5497246451155324</v>
       </c>
       <c r="L176" t="n">
         <v>1.1875</v>
@@ -24793,7 +24793,7 @@
         <v>-0.18465227817745797</v>
       </c>
       <c r="AC176" t="n">
-        <v>-0.5689655172413792</v>
+        <v>-0.5689655172413799</v>
       </c>
       <c r="AD176"/>
       <c r="AE176" t="n">
@@ -24997,7 +24997,7 @@
         <v>0.5542929292929293</v>
       </c>
       <c r="K178" t="n">
-        <v>0.7437212953676028</v>
+        <v>0.7437212953676031</v>
       </c>
       <c r="L178" t="n">
         <v>1.8518518518518519</v>
@@ -25126,7 +25126,7 @@
         <v>0.6785009861932939</v>
       </c>
       <c r="K179" t="n">
-        <v>0.7872163097076944</v>
+        <v>0.7872163097076946</v>
       </c>
       <c r="L179" t="n">
         <v>1.4782608695652173</v>
@@ -25180,7 +25180,7 @@
         <v>-0.5433070866141727</v>
       </c>
       <c r="AC179" t="n">
-        <v>-0.5555555555555555</v>
+        <v>-0.555555555555555</v>
       </c>
       <c r="AD179"/>
       <c r="AE179" t="n">
@@ -25255,7 +25255,7 @@
         <v>0.6033057851239669</v>
       </c>
       <c r="K180" t="n">
-        <v>0.7286742057325313</v>
+        <v>0.7286742057325312</v>
       </c>
       <c r="L180" t="n">
         <v>1.5238095238095237</v>
@@ -25309,7 +25309,7 @@
         <v>-0.29729729729729704</v>
       </c>
       <c r="AC180" t="n">
-        <v>-0.8607594936708863</v>
+        <v>-0.8607594936708868</v>
       </c>
       <c r="AD180" t="n">
         <v>2.0</v>
@@ -25384,7 +25384,7 @@
         <v>0.6484375</v>
       </c>
       <c r="K181" t="n">
-        <v>0.667596046705959</v>
+        <v>0.6675960467059586</v>
       </c>
       <c r="L181" t="n">
         <v>3.5483870967741935</v>
@@ -25513,7 +25513,7 @@
         <v>0.5795454545454546</v>
       </c>
       <c r="K182" t="n">
-        <v>0.5876751203535707</v>
+        <v>0.5876751203535705</v>
       </c>
       <c r="L182" t="n">
         <v>1.4</v>
@@ -25567,7 +25567,7 @@
         <v>-0.6000000000000001</v>
       </c>
       <c r="AC182" t="n">
-        <v>-0.9882491186839014</v>
+        <v>-0.9882491186839015</v>
       </c>
       <c r="AD182"/>
       <c r="AE182" t="n">
@@ -25696,7 +25696,7 @@
         <v>0.21348314606741464</v>
       </c>
       <c r="AC183" t="n">
-        <v>-0.9398998330550921</v>
+        <v>-0.9398998330550923</v>
       </c>
       <c r="AD183"/>
       <c r="AE183" t="n">
@@ -25771,7 +25771,7 @@
         <v>0.6256354393609296</v>
       </c>
       <c r="K184" t="n">
-        <v>0.7750910953322785</v>
+        <v>0.7750910953322778</v>
       </c>
       <c r="L184" t="n">
         <v>1.8545454545454545</v>
@@ -25825,7 +25825,7 @@
         <v>-0.344051446945338</v>
       </c>
       <c r="AC184" t="n">
-        <v>-0.6582840236686389</v>
+        <v>-0.6582840236686387</v>
       </c>
       <c r="AD184"/>
       <c r="AE184" t="n">
@@ -25900,7 +25900,7 @@
         <v>0.5498737373737373</v>
       </c>
       <c r="K185" t="n">
-        <v>0.5921570582603477</v>
+        <v>0.5921570582603475</v>
       </c>
       <c r="L185" t="n">
         <v>1.6153846153846154</v>
@@ -26029,7 +26029,7 @@
         <v>0.6400394477317555</v>
       </c>
       <c r="K186" t="n">
-        <v>0.7085243743539135</v>
+        <v>0.7085243743539138</v>
       </c>
       <c r="L186" t="n">
         <v>2.230769230769231</v>
@@ -26083,7 +26083,7 @@
         <v>0.8461538461538467</v>
       </c>
       <c r="AC186" t="n">
-        <v>-0.9753381066030233</v>
+        <v>-0.9753381066030232</v>
       </c>
       <c r="AD186"/>
       <c r="AE186" t="n">
@@ -26287,7 +26287,7 @@
         <v>0.41020408163265304</v>
       </c>
       <c r="K188" t="n">
-        <v>0.651186254450461</v>
+        <v>0.651186254450463</v>
       </c>
       <c r="L188" t="n">
         <v>3.619047619047619</v>
@@ -26341,7 +26341,7 @@
         <v>0.5995232419547062</v>
       </c>
       <c r="AC188" t="n">
-        <v>-0.48453608247422636</v>
+        <v>-0.4845360824742277</v>
       </c>
       <c r="AD188" t="n">
         <v>2.0</v>
@@ -26416,7 +26416,7 @@
         <v>0.543171114599686</v>
       </c>
       <c r="K189" t="n">
-        <v>0.6153114420716119</v>
+        <v>0.6153114420716117</v>
       </c>
       <c r="L189" t="n">
         <v>3.0</v>
@@ -26470,7 +26470,7 @@
         <v>-0.029411764705882693</v>
       </c>
       <c r="AC189" t="n">
-        <v>-0.5115044247787612</v>
+        <v>-0.5115044247787609</v>
       </c>
       <c r="AD189" t="n">
         <v>2.0</v>
@@ -26545,7 +26545,7 @@
         <v>0.48547979797979796</v>
       </c>
       <c r="K190" t="n">
-        <v>0.6210125873430767</v>
+        <v>0.6210125873430768</v>
       </c>
       <c r="L190" t="n">
         <v>3.2790697674418605</v>
@@ -26599,7 +26599,7 @@
         <v>0.02094240837696234</v>
       </c>
       <c r="AC190" t="n">
-        <v>-0.5857338820301784</v>
+        <v>-0.5857338820301771</v>
       </c>
       <c r="AD190" t="n">
         <v>7.0</v>
@@ -26674,7 +26674,7 @@
         <v>0.5887573964497042</v>
       </c>
       <c r="K191" t="n">
-        <v>0.6599557056359688</v>
+        <v>0.6599557056359696</v>
       </c>
       <c r="L191" t="n">
         <v>1.6774193548387097</v>
@@ -26803,7 +26803,7 @@
         <v>0.7000726216412491</v>
       </c>
       <c r="K192" t="n">
-        <v>0.7917764071627923</v>
+        <v>0.7917764071627925</v>
       </c>
       <c r="L192" t="n">
         <v>2.176470588235294</v>
@@ -26932,7 +26932,7 @@
         <v>0.4939682539682539</v>
       </c>
       <c r="K193" t="n">
-        <v>0.6190775915470379</v>
+        <v>0.6190775915470377</v>
       </c>
       <c r="L193" t="n">
         <v>5.948717948717949</v>
@@ -26986,7 +26986,7 @@
         <v>0.2802768166089978</v>
       </c>
       <c r="AC193" t="n">
-        <v>-0.5082872928176795</v>
+        <v>-0.5082872928176803</v>
       </c>
       <c r="AD193" t="n">
         <v>2.0</v>
@@ -27061,7 +27061,7 @@
         <v>0.6457142857142857</v>
       </c>
       <c r="K194" t="n">
-        <v>0.6386654272696458</v>
+        <v>0.6386654272696457</v>
       </c>
       <c r="L194" t="n">
         <v>1.9807692307692308</v>
@@ -27115,7 +27115,7 @@
         <v>-0.226792009400705</v>
       </c>
       <c r="AC194" t="n">
-        <v>-0.8163934426229507</v>
+        <v>-0.8163934426229515</v>
       </c>
       <c r="AD194" t="n">
         <v>2.0</v>
@@ -27190,7 +27190,7 @@
         <v>0.5266875981161695</v>
       </c>
       <c r="K195" t="n">
-        <v>0.6984699014959428</v>
+        <v>0.6984699014959431</v>
       </c>
       <c r="L195" t="n">
         <v>3.409090909090909</v>
@@ -27319,7 +27319,7 @@
         <v>0.47534516765285995</v>
       </c>
       <c r="K196" t="n">
-        <v>0.5801949258430951</v>
+        <v>0.5801949258430953</v>
       </c>
       <c r="L196" t="n">
         <v>2.5</v>
@@ -27373,7 +27373,7 @@
         <v>0.5243902439024392</v>
       </c>
       <c r="AC196" t="n">
-        <v>-0.352</v>
+        <v>-0.3519999999999992</v>
       </c>
       <c r="AD196" t="n">
         <v>3.0</v>
@@ -27448,7 +27448,7 @@
         <v>0.6264462809917355</v>
       </c>
       <c r="K197" t="n">
-        <v>0.6813106699907031</v>
+        <v>0.6813106699907033</v>
       </c>
       <c r="L197" t="n">
         <v>1.631578947368421</v>
@@ -27502,7 +27502,7 @@
         <v>0.32653061224489777</v>
       </c>
       <c r="AC197" t="n">
-        <v>-0.4903225806451612</v>
+        <v>-0.4903225806451609</v>
       </c>
       <c r="AD197" t="n">
         <v>4.0</v>
@@ -27575,7 +27575,7 @@
         <v>0.5053968253968254</v>
       </c>
       <c r="K198" t="n">
-        <v>0.5950426851247089</v>
+        <v>0.5950426851247096</v>
       </c>
       <c r="L198" t="n">
         <v>1.8055555555555556</v>
@@ -27629,7 +27629,7 @@
         <v>0.4685990338164253</v>
       </c>
       <c r="AC198" t="n">
-        <v>-0.6973684210526319</v>
+        <v>-0.6973684210526307</v>
       </c>
       <c r="AD198" t="n">
         <v>2.0</v>
@@ -27704,7 +27704,7 @@
         <v>0.5703125</v>
       </c>
       <c r="K199" t="n">
-        <v>0.712421535363471</v>
+        <v>0.7124215353634707</v>
       </c>
       <c r="L199" t="n">
         <v>3.7413793103448274</v>
@@ -27833,7 +27833,7 @@
         <v>0.727810650887574</v>
       </c>
       <c r="K200" t="n">
-        <v>0.7451447138637767</v>
+        <v>0.7451447138637768</v>
       </c>
       <c r="L200" t="n">
         <v>4.029411764705882</v>
@@ -27887,7 +27887,7 @@
         <v>-0.5664335664335659</v>
       </c>
       <c r="AC200" t="n">
-        <v>-0.841441441441441</v>
+        <v>-0.8414414414414413</v>
       </c>
       <c r="AD200" t="n">
         <v>2.0</v>
@@ -27962,7 +27962,7 @@
         <v>0.6229166666666667</v>
       </c>
       <c r="K201" t="n">
-        <v>0.6444444444444446</v>
+        <v>0.6444444444444445</v>
       </c>
       <c r="L201" t="n">
         <v>2.186046511627907</v>
@@ -28091,7 +28091,7 @@
         <v>0.6400394477317555</v>
       </c>
       <c r="K202" t="n">
-        <v>0.7085243743539135</v>
+        <v>0.7085243743539134</v>
       </c>
       <c r="L202" t="n">
         <v>1.6176470588235294</v>
@@ -28145,7 +28145,7 @@
         <v>-0.621505376344086</v>
       </c>
       <c r="AC202" t="n">
-        <v>-0.9753381066030233</v>
+        <v>-0.9753381066030232</v>
       </c>
       <c r="AD202" t="n">
         <v>2.0</v>
@@ -28220,7 +28220,7 @@
         <v>0.6057142857142858</v>
       </c>
       <c r="K203" t="n">
-        <v>0.6792023205240193</v>
+        <v>0.6792023205240192</v>
       </c>
       <c r="L203" t="n">
         <v>1.9795918367346939</v>
@@ -28274,7 +28274,7 @@
         <v>0.14572864321607903</v>
       </c>
       <c r="AC203" t="n">
-        <v>-0.9825857519788921</v>
+        <v>-0.9825857519788919</v>
       </c>
       <c r="AD203" t="n">
         <v>2.0</v>
@@ -28403,7 +28403,7 @@
         <v>0.5966386554621839</v>
       </c>
       <c r="AC204" t="n">
-        <v>-0.9882491186839014</v>
+        <v>-0.9882491186839015</v>
       </c>
       <c r="AD204" t="n">
         <v>2.0</v>
@@ -28532,7 +28532,7 @@
         <v>-0.590361445783132</v>
       </c>
       <c r="AC205" t="n">
-        <v>-0.9224489795918367</v>
+        <v>-0.9224489795918362</v>
       </c>
       <c r="AD205" t="n">
         <v>2.0</v>
@@ -28607,7 +28607,7 @@
         <v>0.48226643598615915</v>
       </c>
       <c r="K206" t="n">
-        <v>0.668415633175815</v>
+        <v>0.6684156331758151</v>
       </c>
       <c r="L206" t="n">
         <v>1.7272727272727273</v>
@@ -28661,7 +28661,7 @@
         <v>-0.0982658959537569</v>
       </c>
       <c r="AC206" t="n">
-        <v>-0.4704347826086959</v>
+        <v>-0.4704347826086963</v>
       </c>
       <c r="AD206" t="n">
         <v>2.0</v>
@@ -28790,7 +28790,7 @@
         <v>-0.5826086956521729</v>
       </c>
       <c r="AC207" t="n">
-        <v>-0.7682811016144351</v>
+        <v>-0.7682811016144352</v>
       </c>
       <c r="AD207" t="n">
         <v>2.0</v>
@@ -28865,7 +28865,7 @@
         <v>0.7256671899529042</v>
       </c>
       <c r="K208" t="n">
-        <v>0.6975176159222338</v>
+        <v>0.6975176159222342</v>
       </c>
       <c r="L208" t="n">
         <v>1.56</v>
@@ -28919,7 +28919,7 @@
         <v>0.30232558139534954</v>
       </c>
       <c r="AC208" t="n">
-        <v>-0.6489151873767258</v>
+        <v>-0.6489151873767263</v>
       </c>
       <c r="AD208" t="n">
         <v>2.0</v>
@@ -28994,7 +28994,7 @@
         <v>0.5619791666666667</v>
       </c>
       <c r="K209" t="n">
-        <v>0.6431061396231921</v>
+        <v>0.6431061396231923</v>
       </c>
       <c r="L209" t="n">
         <v>1.7714285714285714</v>
@@ -29123,7 +29123,7 @@
         <v>0.37247474747474746</v>
       </c>
       <c r="K210" t="n">
-        <v>0.583906988326783</v>
+        <v>0.5839069883267833</v>
       </c>
       <c r="L210" t="n">
         <v>1.7727272727272727</v>
@@ -29177,7 +29177,7 @@
         <v>0.45864661654135314</v>
       </c>
       <c r="AC210" t="n">
-        <v>-0.4237288135593215</v>
+        <v>-0.42372881355932407</v>
       </c>
       <c r="AD210" t="n">
         <v>2.0</v>
@@ -29252,7 +29252,7 @@
         <v>0.5996055226824457</v>
       </c>
       <c r="K211" t="n">
-        <v>0.6337316859671387</v>
+        <v>0.633731685967139</v>
       </c>
       <c r="L211" t="n">
         <v>1.4166666666666667</v>
@@ -29306,7 +29306,7 @@
         <v>0.07894736842105296</v>
       </c>
       <c r="AC211" t="n">
-        <v>-0.8156028368794326</v>
+        <v>-0.8156028368794329</v>
       </c>
       <c r="AD211" t="n">
         <v>2.0</v>
@@ -29435,7 +29435,7 @@
         <v>0.8656126482213412</v>
       </c>
       <c r="AC212" t="n">
-        <v>-0.7856910569105692</v>
+        <v>-0.7856910569105687</v>
       </c>
       <c r="AD212" t="n">
         <v>2.0</v>
@@ -29510,7 +29510,7 @@
         <v>0.8386678200692042</v>
       </c>
       <c r="K213" t="n">
-        <v>0.8259313085580422</v>
+        <v>0.8259313085580421</v>
       </c>
       <c r="L213" t="n">
         <v>1.706896551724138</v>
@@ -29564,7 +29564,7 @@
         <v>-0.8172983479105936</v>
       </c>
       <c r="AC213" t="n">
-        <v>-0.7980309423347397</v>
+        <v>-0.7980309423347396</v>
       </c>
       <c r="AD213" t="n">
         <v>2.0</v>
@@ -29639,7 +29639,7 @@
         <v>0.6692063492063492</v>
       </c>
       <c r="K214" t="n">
-        <v>0.7297654917292115</v>
+        <v>0.7297654917292117</v>
       </c>
       <c r="L214" t="n">
         <v>2.5238095238095237</v>
@@ -29768,7 +29768,7 @@
         <v>0.6805555555555556</v>
       </c>
       <c r="K215" t="n">
-        <v>0.7503994041344023</v>
+        <v>0.7503994041344021</v>
       </c>
       <c r="L215" t="n">
         <v>2.590909090909091</v>
@@ -29822,7 +29822,7 @@
         <v>-0.615384615384616</v>
       </c>
       <c r="AC215" t="n">
-        <v>-0.9224489795918367</v>
+        <v>-0.9224489795918362</v>
       </c>
       <c r="AD215" t="n">
         <v>2.0</v>
@@ -29897,7 +29897,7 @@
         <v>0.4913657770800628</v>
       </c>
       <c r="K216" t="n">
-        <v>0.646661226435627</v>
+        <v>0.6466612264356273</v>
       </c>
       <c r="L216" t="n">
         <v>1.44</v>
@@ -30080,7 +30080,7 @@
         <v>0.6296296296296294</v>
       </c>
       <c r="AC217" t="n">
-        <v>-0.6577181208053691</v>
+        <v>-0.6577181208053687</v>
       </c>
       <c r="AD217" t="n">
         <v>2.0</v>

</xml_diff>